<commit_message>
Daily scrum anggota. Scrummaster : Leni
</commit_message>
<xml_diff>
--- a/src/log-book/LogBook-speaker-team.xlsx
+++ b/src/log-book/LogBook-speaker-team.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TI-D pagi (MIKROSKIL)\semester-4\TKPPPL\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Informasi Umum" sheetId="1" r:id="rId1"/>
@@ -28,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="96">
   <si>
     <t>Nama kelompok</t>
   </si>
@@ -241,6 +236,81 @@
   </si>
   <si>
     <t>1. Mengaktifkan grunt server</t>
+  </si>
+  <si>
+    <t>DAILY SCRUM 05 JUNI / 10 JUNI</t>
+  </si>
+  <si>
+    <t>Scrummaster : Leni Hadianti</t>
+  </si>
+  <si>
+    <t>1. Kemarin saya               :</t>
+  </si>
+  <si>
+    <t>1. Menggunakan kembali file Harisu yang sempat di keluarkan dari daftar Trasngender</t>
+  </si>
+  <si>
+    <t>local server error</t>
+  </si>
+  <si>
+    <t>1. Mengumpulkan informasi tentang Dena Rachman (Salah satu pria transgender)</t>
+  </si>
+  <si>
+    <t>1. Membuat kerangka HTML di dalam index.jade</t>
+  </si>
+  <si>
+    <t>pull request yang merging dari anggota lain</t>
+  </si>
+  <si>
+    <t>1. Memperbaiki index.jade yang error dalam github</t>
+  </si>
+  <si>
+    <t>2. Memperbaiki pull request yang merging</t>
+  </si>
+  <si>
+    <t>3. Push commit index.jade yang selesai di perbaiki</t>
+  </si>
+  <si>
+    <t>1. Memperbarui isi daily scrum</t>
+  </si>
+  <si>
+    <t>Local server error</t>
+  </si>
+  <si>
+    <t>1. Cari tahu bagaimana cara menyelipkan image ke dalam dile index.jade</t>
+  </si>
+  <si>
+    <t>2. Membuat kerangka HTML di dalam index.jade</t>
+  </si>
+  <si>
+    <t>4. Memperbarui isi daily scrum</t>
+  </si>
+  <si>
+    <t>Grunt server tidak terbuka</t>
+  </si>
+  <si>
+    <t>2. Memperbarui isi daily scrum</t>
+  </si>
+  <si>
+    <t>1. Mengumpulkan informasi tentang Alicia Liu</t>
+  </si>
+  <si>
+    <t>sintaks error jade</t>
+  </si>
+  <si>
+    <t>1. Mengumpulkan informasi tentang Florencia De La V (Salah satu pria transgender)</t>
+  </si>
+  <si>
+    <t>pull request</t>
+  </si>
+  <si>
+    <t>1. Mencari tahu bagaimana cara menyelipkan image ke dalam file index .jade</t>
+  </si>
+  <si>
+    <t>2. Membut kerangka HTML di dalam index.jade</t>
+  </si>
+  <si>
+    <t>3. Membuat cover perkenalan nama kelompok ke dalam slide bespoke (jade)</t>
   </si>
 </sst>
 </file>
@@ -330,7 +400,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -379,8 +449,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -493,11 +569,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -547,6 +634,49 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="11" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="3" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="3" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -559,36 +689,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -607,18 +707,18 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -640,19 +740,55 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="16" fontId="11" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="3" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="3" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -713,7 +849,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -748,7 +884,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -925,7 +1061,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -947,99 +1083,99 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="33" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-      <c r="K1" s="26"/>
-      <c r="L1" s="26"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
+      <c r="L1" s="24"/>
     </row>
     <row r="2" spans="1:12" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="27" t="s">
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
-      <c r="J2" s="27"/>
-      <c r="K2" s="27"/>
-      <c r="L2" s="27"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
+      <c r="K2" s="25"/>
+      <c r="L2" s="25"/>
     </row>
     <row r="3" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="31" t="s">
+      <c r="A3" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="31"/>
-      <c r="C3" s="31"/>
-      <c r="D3" s="32" t="s">
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
-      <c r="K3" s="32"/>
-      <c r="L3" s="32"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="33"/>
+      <c r="I3" s="33"/>
+      <c r="J3" s="33"/>
+      <c r="K3" s="33"/>
+      <c r="L3" s="33"/>
     </row>
     <row r="4" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="28" t="s">
+      <c r="B4" s="32"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="28"/>
-      <c r="F4" s="28"/>
-      <c r="G4" s="28"/>
-      <c r="H4" s="28"/>
-      <c r="I4" s="28"/>
-      <c r="J4" s="28"/>
-      <c r="K4" s="28"/>
-      <c r="L4" s="28"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="26"/>
+      <c r="H4" s="26"/>
+      <c r="I4" s="26"/>
+      <c r="J4" s="26"/>
+      <c r="K4" s="26"/>
+      <c r="L4" s="26"/>
     </row>
     <row r="5" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="31" t="s">
+      <c r="A5" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="31"/>
-      <c r="C5" s="31"/>
-      <c r="D5" s="28" t="s">
+      <c r="B5" s="32"/>
+      <c r="C5" s="32"/>
+      <c r="D5" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="28"/>
-      <c r="F5" s="28"/>
-      <c r="G5" s="28"/>
-      <c r="H5" s="28"/>
-      <c r="I5" s="28"/>
-      <c r="J5" s="28"/>
-      <c r="K5" s="28"/>
-      <c r="L5" s="28"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="26"/>
+      <c r="H5" s="26"/>
+      <c r="I5" s="26"/>
+      <c r="J5" s="26"/>
+      <c r="K5" s="26"/>
+      <c r="L5" s="26"/>
     </row>
     <row r="6" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="29" t="s">
+      <c r="A6" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="30"/>
-      <c r="C6" s="30"/>
+      <c r="B6" s="28"/>
+      <c r="C6" s="28"/>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
       <c r="F6" s="11"/>
@@ -1048,7 +1184,7 @@
       <c r="I6" s="11"/>
       <c r="J6" s="11"/>
       <c r="K6" s="11"/>
-      <c r="L6" s="22"/>
+      <c r="L6" s="37"/>
     </row>
     <row r="7" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A7" s="12"/>
@@ -1056,17 +1192,17 @@
         <v>6</v>
       </c>
       <c r="C7" s="11"/>
-      <c r="D7" s="25" t="s">
+      <c r="D7" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="25"/>
+      <c r="E7" s="31"/>
       <c r="F7" s="11"/>
       <c r="G7" s="11"/>
       <c r="H7" s="11"/>
       <c r="I7" s="11"/>
       <c r="J7" s="11"/>
       <c r="K7" s="11"/>
-      <c r="L7" s="22"/>
+      <c r="L7" s="37"/>
     </row>
     <row r="8" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A8" s="12"/>
@@ -1074,24 +1210,24 @@
         <v>7</v>
       </c>
       <c r="C8" s="11"/>
-      <c r="D8" s="25">
+      <c r="D8" s="31">
         <v>121112295</v>
       </c>
-      <c r="E8" s="25"/>
+      <c r="E8" s="31"/>
       <c r="F8" s="11"/>
       <c r="G8" s="11"/>
       <c r="H8" s="11"/>
       <c r="I8" s="11"/>
       <c r="J8" s="11"/>
       <c r="K8" s="11"/>
-      <c r="L8" s="22"/>
+      <c r="L8" s="37"/>
     </row>
     <row r="9" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="23" t="s">
+      <c r="A9" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="24"/>
-      <c r="C9" s="24"/>
+      <c r="B9" s="30"/>
+      <c r="C9" s="30"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
       <c r="F9" s="11"/>
@@ -1100,7 +1236,7 @@
       <c r="I9" s="11"/>
       <c r="J9" s="11"/>
       <c r="K9" s="11"/>
-      <c r="L9" s="22"/>
+      <c r="L9" s="37"/>
     </row>
     <row r="10" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A10" s="12"/>
@@ -1108,17 +1244,17 @@
         <v>6</v>
       </c>
       <c r="C10" s="11"/>
-      <c r="D10" s="25" t="s">
+      <c r="D10" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="25"/>
+      <c r="E10" s="31"/>
       <c r="F10" s="11"/>
       <c r="G10" s="11"/>
       <c r="H10" s="11"/>
       <c r="I10" s="11"/>
       <c r="J10" s="11"/>
       <c r="K10" s="11"/>
-      <c r="L10" s="22"/>
+      <c r="L10" s="37"/>
     </row>
     <row r="11" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A11" s="12"/>
@@ -1126,24 +1262,24 @@
         <v>7</v>
       </c>
       <c r="C11" s="11"/>
-      <c r="D11" s="25">
+      <c r="D11" s="31">
         <v>121112911</v>
       </c>
-      <c r="E11" s="25"/>
+      <c r="E11" s="31"/>
       <c r="F11" s="11"/>
       <c r="G11" s="11"/>
       <c r="H11" s="11"/>
       <c r="I11" s="11"/>
       <c r="J11" s="11"/>
       <c r="K11" s="11"/>
-      <c r="L11" s="22"/>
+      <c r="L11" s="37"/>
     </row>
     <row r="12" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="23" t="s">
+      <c r="A12" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="24"/>
-      <c r="C12" s="24"/>
+      <c r="B12" s="30"/>
+      <c r="C12" s="30"/>
       <c r="D12" s="11"/>
       <c r="E12" s="11"/>
       <c r="F12" s="11"/>
@@ -1152,7 +1288,7 @@
       <c r="I12" s="11"/>
       <c r="J12" s="11"/>
       <c r="K12" s="11"/>
-      <c r="L12" s="22"/>
+      <c r="L12" s="37"/>
     </row>
     <row r="13" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A13" s="11"/>
@@ -1160,17 +1296,17 @@
         <v>6</v>
       </c>
       <c r="C13" s="11"/>
-      <c r="D13" s="25" t="s">
+      <c r="D13" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="E13" s="25"/>
+      <c r="E13" s="31"/>
       <c r="F13" s="11"/>
       <c r="G13" s="11"/>
       <c r="H13" s="11"/>
       <c r="I13" s="11"/>
       <c r="J13" s="11"/>
       <c r="K13" s="11"/>
-      <c r="L13" s="22"/>
+      <c r="L13" s="37"/>
     </row>
     <row r="14" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A14" s="11"/>
@@ -1178,34 +1314,41 @@
         <v>7</v>
       </c>
       <c r="C14" s="11"/>
-      <c r="D14" s="25">
+      <c r="D14" s="31">
         <v>121112724</v>
       </c>
-      <c r="E14" s="25"/>
+      <c r="E14" s="31"/>
       <c r="F14" s="11"/>
       <c r="G14" s="11"/>
       <c r="H14" s="11"/>
       <c r="I14" s="11"/>
       <c r="J14" s="11"/>
       <c r="K14" s="11"/>
-      <c r="L14" s="22"/>
+      <c r="L14" s="37"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="19"/>
-      <c r="B15" s="20"/>
-      <c r="C15" s="20"/>
-      <c r="D15" s="20"/>
-      <c r="E15" s="20"/>
-      <c r="F15" s="20"/>
-      <c r="G15" s="20"/>
-      <c r="H15" s="20"/>
-      <c r="I15" s="20"/>
-      <c r="J15" s="20"/>
-      <c r="K15" s="20"/>
-      <c r="L15" s="21"/>
+      <c r="A15" s="34"/>
+      <c r="B15" s="35"/>
+      <c r="C15" s="35"/>
+      <c r="D15" s="35"/>
+      <c r="E15" s="35"/>
+      <c r="F15" s="35"/>
+      <c r="G15" s="35"/>
+      <c r="H15" s="35"/>
+      <c r="I15" s="35"/>
+      <c r="J15" s="35"/>
+      <c r="K15" s="35"/>
+      <c r="L15" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A15:L15"/>
+    <mergeCell ref="L6:L14"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D14:E14"/>
     <mergeCell ref="A1:L1"/>
     <mergeCell ref="D2:L2"/>
     <mergeCell ref="D4:L4"/>
@@ -1219,13 +1362,6 @@
     <mergeCell ref="A5:C5"/>
     <mergeCell ref="D5:L5"/>
     <mergeCell ref="D3:L3"/>
-    <mergeCell ref="A15:L15"/>
-    <mergeCell ref="L6:L14"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D14:E14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1249,125 +1385,125 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="35"/>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="40"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="43" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
       <c r="D2" s="3"/>
-      <c r="E2" s="35"/>
+      <c r="E2" s="40"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="35"/>
+      <c r="B3" s="42"/>
+      <c r="C3" s="42"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="40"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="37" t="s">
+      <c r="A4" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="37"/>
+      <c r="B4" s="42"/>
       <c r="C4" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D4" s="3">
         <v>121112295</v>
       </c>
-      <c r="E4" s="35"/>
+      <c r="E4" s="40"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="38" t="s">
+      <c r="A5" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="38"/>
-      <c r="C5" s="38"/>
+      <c r="B5" s="43"/>
+      <c r="C5" s="43"/>
       <c r="D5" s="3"/>
-      <c r="E5" s="35"/>
+      <c r="E5" s="40"/>
     </row>
     <row r="6" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="37" t="s">
+      <c r="A6" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="37"/>
-      <c r="C6" s="37"/>
-      <c r="D6" s="37"/>
-      <c r="E6" s="35"/>
+      <c r="B6" s="42"/>
+      <c r="C6" s="42"/>
+      <c r="D6" s="42"/>
+      <c r="E6" s="40"/>
     </row>
     <row r="7" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="37" t="s">
+      <c r="A7" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="37"/>
+      <c r="B7" s="42"/>
       <c r="C7" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D7" s="3">
         <v>121112911</v>
       </c>
-      <c r="E7" s="35"/>
+      <c r="E7" s="40"/>
     </row>
     <row r="8" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="38" t="s">
+      <c r="A8" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="38"/>
-      <c r="C8" s="38"/>
+      <c r="B8" s="43"/>
+      <c r="C8" s="43"/>
       <c r="D8" s="3"/>
-      <c r="E8" s="35"/>
+      <c r="E8" s="40"/>
     </row>
     <row r="9" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="37" t="s">
+      <c r="A9" s="42" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="37"/>
-      <c r="C9" s="37"/>
-      <c r="D9" s="37"/>
-      <c r="E9" s="35"/>
+      <c r="B9" s="42"/>
+      <c r="C9" s="42"/>
+      <c r="D9" s="42"/>
+      <c r="E9" s="40"/>
     </row>
     <row r="10" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="37" t="s">
+      <c r="A10" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="37"/>
+      <c r="B10" s="42"/>
       <c r="C10" s="3" t="s">
         <v>15</v>
       </c>
       <c r="D10" s="3">
         <v>121112724</v>
       </c>
-      <c r="E10" s="35"/>
+      <c r="E10" s="40"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="33"/>
-      <c r="B11" s="33"/>
-      <c r="C11" s="33"/>
-      <c r="D11" s="34"/>
-      <c r="E11" s="35"/>
+      <c r="A11" s="38"/>
+      <c r="B11" s="38"/>
+      <c r="C11" s="38"/>
+      <c r="D11" s="39"/>
+      <c r="E11" s="40"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -1390,10 +1526,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I33"/>
+  <dimension ref="A1:I62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="B59" sqref="B59:D59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1402,26 +1538,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
       <c r="F1" s="8"/>
       <c r="G1" s="8"/>
       <c r="H1" s="8"/>
       <c r="I1" s="8"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="42" t="s">
+      <c r="A2" s="44" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="42"/>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
+      <c r="B2" s="44"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="45"/>
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
     </row>
@@ -1435,11 +1571,11 @@
     </row>
     <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="6"/>
-      <c r="B4" s="41" t="s">
+      <c r="B4" s="46" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="41"/>
-      <c r="D4" s="41"/>
+      <c r="C4" s="46"/>
+      <c r="D4" s="46"/>
       <c r="E4" t="s">
         <v>31</v>
       </c>
@@ -1464,11 +1600,11 @@
     </row>
     <row r="7" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
-      <c r="B7" s="41" t="s">
+      <c r="B7" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="41"/>
-      <c r="D7" s="41"/>
+      <c r="C7" s="46"/>
+      <c r="D7" s="46"/>
       <c r="E7" t="s">
         <v>32</v>
       </c>
@@ -1503,11 +1639,11 @@
     </row>
     <row r="11" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
-      <c r="B11" s="41" t="s">
+      <c r="B11" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="41"/>
-      <c r="D11" s="41"/>
+      <c r="C11" s="46"/>
+      <c r="D11" s="46"/>
       <c r="E11" t="s">
         <v>33</v>
       </c>
@@ -1541,11 +1677,11 @@
     </row>
     <row r="15" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="6"/>
-      <c r="B15" s="41" t="s">
+      <c r="B15" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="C15" s="41"/>
-      <c r="D15" s="41"/>
+      <c r="C15" s="46"/>
+      <c r="D15" s="46"/>
       <c r="E15" t="s">
         <v>49</v>
       </c>
@@ -1598,11 +1734,11 @@
     </row>
     <row r="21" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="6"/>
-      <c r="B21" s="41" t="s">
+      <c r="B21" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="C21" s="41"/>
-      <c r="D21" s="41"/>
+      <c r="C21" s="46"/>
+      <c r="D21" s="46"/>
       <c r="E21" t="s">
         <v>45</v>
       </c>
@@ -1627,11 +1763,11 @@
     </row>
     <row r="24" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="6"/>
-      <c r="B24" s="41" t="s">
+      <c r="B24" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="C24" s="41"/>
-      <c r="D24" s="41"/>
+      <c r="C24" s="46"/>
+      <c r="D24" s="46"/>
       <c r="E24" t="s">
         <v>44</v>
       </c>
@@ -1684,11 +1820,11 @@
     </row>
     <row r="30" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="5"/>
-      <c r="B30" s="41" t="s">
+      <c r="B30" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="C30" s="41"/>
-      <c r="D30" s="41"/>
+      <c r="C30" s="46"/>
+      <c r="D30" s="46"/>
       <c r="E30" t="s">
         <v>47</v>
       </c>
@@ -1713,28 +1849,305 @@
     </row>
     <row r="33" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="5"/>
-      <c r="B33" s="39" t="s">
+      <c r="B33" s="45" t="s">
         <v>30</v>
       </c>
-      <c r="C33" s="39"/>
-      <c r="D33" s="39"/>
+      <c r="C33" s="45"/>
+      <c r="D33" s="45"/>
       <c r="E33" t="s">
         <v>32</v>
       </c>
     </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="56" t="s">
+        <v>71</v>
+      </c>
+      <c r="B35" s="56"/>
+      <c r="C35" s="56"/>
+      <c r="D35" s="56"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="57" t="s">
+        <v>72</v>
+      </c>
+      <c r="B36" s="57"/>
+      <c r="C36" s="57"/>
+      <c r="D36" s="57"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="58">
+        <v>41796</v>
+      </c>
+      <c r="B37" s="59"/>
+      <c r="C37" s="60"/>
+      <c r="D37" s="60"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="60"/>
+      <c r="B38" s="61" t="s">
+        <v>73</v>
+      </c>
+      <c r="C38" s="61"/>
+      <c r="D38" s="61"/>
+      <c r="E38" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="60"/>
+      <c r="B39" s="60"/>
+      <c r="C39" s="60"/>
+      <c r="D39" s="60"/>
+      <c r="E39" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="60"/>
+      <c r="B40" s="60"/>
+      <c r="C40" s="60"/>
+      <c r="D40" s="60"/>
+      <c r="E40" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="60"/>
+      <c r="B41" s="61" t="s">
+        <v>29</v>
+      </c>
+      <c r="C41" s="61"/>
+      <c r="D41" s="61"/>
+      <c r="E41" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="60"/>
+      <c r="B42" s="60"/>
+      <c r="C42" s="60"/>
+      <c r="D42" s="60"/>
+      <c r="E42" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="60"/>
+      <c r="B43" s="61" t="s">
+        <v>30</v>
+      </c>
+      <c r="C43" s="61"/>
+      <c r="D43" s="61"/>
+      <c r="E43" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="58">
+        <v>41797</v>
+      </c>
+      <c r="B44" s="60"/>
+      <c r="C44" s="60"/>
+      <c r="D44" s="60"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="60"/>
+      <c r="B45" s="60" t="s">
+        <v>28</v>
+      </c>
+      <c r="C45" s="60"/>
+      <c r="D45" s="60"/>
+      <c r="E45" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E46" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="60"/>
+      <c r="B47" s="61" t="s">
+        <v>29</v>
+      </c>
+      <c r="C47" s="61"/>
+      <c r="D47" s="61"/>
+      <c r="E47" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="60"/>
+      <c r="B48" s="60"/>
+      <c r="C48" s="60"/>
+      <c r="D48" s="60"/>
+      <c r="E48" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="60"/>
+      <c r="B49" s="61" t="s">
+        <v>30</v>
+      </c>
+      <c r="C49" s="61"/>
+      <c r="D49" s="61"/>
+      <c r="E49" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="58">
+        <v>41798</v>
+      </c>
+      <c r="B50" s="60"/>
+      <c r="C50" s="60"/>
+      <c r="D50" s="60"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="60"/>
+      <c r="B51" s="60" t="s">
+        <v>28</v>
+      </c>
+      <c r="C51" s="60"/>
+      <c r="D51" s="60"/>
+      <c r="E51" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="60"/>
+      <c r="B52" s="60"/>
+      <c r="C52" s="60"/>
+      <c r="D52" s="60"/>
+      <c r="E52" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="60"/>
+      <c r="B53" s="61" t="s">
+        <v>29</v>
+      </c>
+      <c r="C53" s="61"/>
+      <c r="D53" s="61"/>
+      <c r="E53" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="60"/>
+      <c r="B54" s="60"/>
+      <c r="C54" s="60"/>
+      <c r="D54" s="60"/>
+      <c r="E54" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="60"/>
+      <c r="B55" s="61" t="s">
+        <v>30</v>
+      </c>
+      <c r="C55" s="61"/>
+      <c r="D55" s="61"/>
+      <c r="E55" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="62">
+        <v>41800</v>
+      </c>
+      <c r="B56" s="63"/>
+      <c r="C56" s="63"/>
+      <c r="D56" s="63"/>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="63"/>
+      <c r="B57" s="60" t="s">
+        <v>28</v>
+      </c>
+      <c r="C57" s="60"/>
+      <c r="D57" s="60"/>
+      <c r="E57" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="63"/>
+      <c r="B58" s="60"/>
+      <c r="C58" s="60"/>
+      <c r="D58" s="60"/>
+      <c r="E58" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" s="63"/>
+      <c r="B59" s="61" t="s">
+        <v>29</v>
+      </c>
+      <c r="C59" s="61"/>
+      <c r="D59" s="61"/>
+      <c r="E59" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" s="63"/>
+      <c r="B60" s="60"/>
+      <c r="C60" s="60"/>
+      <c r="D60" s="60"/>
+      <c r="E60" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" s="63"/>
+      <c r="B61" s="60"/>
+      <c r="C61" s="60"/>
+      <c r="D61" s="60"/>
+      <c r="E61" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" s="59"/>
+      <c r="B62" s="61" t="s">
+        <v>30</v>
+      </c>
+      <c r="C62" s="61"/>
+      <c r="D62" s="61"/>
+      <c r="E62" t="s">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="22">
+    <mergeCell ref="B62:D62"/>
+    <mergeCell ref="B47:D47"/>
+    <mergeCell ref="B49:D49"/>
+    <mergeCell ref="B53:D53"/>
+    <mergeCell ref="B55:D55"/>
+    <mergeCell ref="B59:D59"/>
+    <mergeCell ref="A35:D35"/>
+    <mergeCell ref="A36:D36"/>
+    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="B41:D41"/>
+    <mergeCell ref="B43:D43"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B11:D11"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="B33:D33"/>
     <mergeCell ref="B30:D30"/>
     <mergeCell ref="B15:D15"/>
     <mergeCell ref="B21:D21"/>
     <mergeCell ref="B24:D24"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="B11:D11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1742,29 +2155,29 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M25"/>
+  <dimension ref="A1:M54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28:D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="49" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="46"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="51"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="47" t="s">
+      <c r="A2" s="52" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="48"/>
-      <c r="C2" s="48"/>
-      <c r="D2" s="49"/>
+      <c r="B2" s="53"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="54"/>
     </row>
     <row r="3" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="13">
@@ -1776,58 +2189,58 @@
     </row>
     <row r="4" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="15"/>
-      <c r="B4" s="39" t="s">
+      <c r="B4" s="45" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="39"/>
-      <c r="D4" s="39"/>
-      <c r="E4" s="43" t="s">
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="48" t="s">
         <v>53</v>
       </c>
-      <c r="F4" s="43"/>
-      <c r="G4" s="43"/>
-      <c r="H4" s="43"/>
-      <c r="I4" s="43"/>
-      <c r="J4" s="43"/>
-      <c r="K4" s="43"/>
+      <c r="F4" s="48"/>
+      <c r="G4" s="48"/>
+      <c r="H4" s="48"/>
+      <c r="I4" s="48"/>
+      <c r="J4" s="48"/>
+      <c r="K4" s="48"/>
     </row>
     <row r="5" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="15"/>
-      <c r="E5" s="43" t="s">
+      <c r="E5" s="48" t="s">
         <v>54</v>
       </c>
-      <c r="F5" s="43"/>
-      <c r="G5" s="43"/>
-      <c r="H5" s="43"/>
-      <c r="I5" s="43"/>
-      <c r="J5" s="43"/>
-      <c r="K5" s="43"/>
+      <c r="F5" s="48"/>
+      <c r="G5" s="48"/>
+      <c r="H5" s="48"/>
+      <c r="I5" s="48"/>
+      <c r="J5" s="48"/>
+      <c r="K5" s="48"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E6" s="43" t="s">
+      <c r="E6" s="48" t="s">
         <v>55</v>
       </c>
-      <c r="F6" s="43"/>
-      <c r="G6" s="43"/>
-      <c r="H6" s="43"/>
-      <c r="I6" s="43"/>
-      <c r="J6" s="43"/>
-      <c r="K6" s="43"/>
+      <c r="F6" s="48"/>
+      <c r="G6" s="48"/>
+      <c r="H6" s="48"/>
+      <c r="I6" s="48"/>
+      <c r="J6" s="48"/>
+      <c r="K6" s="48"/>
     </row>
     <row r="7" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B7" s="39" t="s">
+      <c r="B7" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="39"/>
-      <c r="D7" s="39"/>
-      <c r="E7" s="43" t="s">
+      <c r="C7" s="45"/>
+      <c r="D7" s="45"/>
+      <c r="E7" s="48" t="s">
         <v>56</v>
       </c>
-      <c r="F7" s="43"/>
-      <c r="G7" s="43"/>
-      <c r="H7" s="43"/>
-      <c r="I7" s="43"/>
-      <c r="J7" s="43"/>
+      <c r="F7" s="48"/>
+      <c r="G7" s="48"/>
+      <c r="H7" s="48"/>
+      <c r="I7" s="48"/>
+      <c r="J7" s="48"/>
     </row>
     <row r="8" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="13">
@@ -1840,37 +2253,37 @@
       </c>
       <c r="C9" s="15"/>
       <c r="D9" s="15"/>
-      <c r="E9" s="43" t="s">
+      <c r="E9" s="48" t="s">
         <v>53</v>
       </c>
-      <c r="F9" s="43"/>
-      <c r="G9" s="43"/>
-      <c r="H9" s="43"/>
-      <c r="I9" s="43"/>
-      <c r="J9" s="43"/>
-      <c r="K9" s="43"/>
+      <c r="F9" s="48"/>
+      <c r="G9" s="48"/>
+      <c r="H9" s="48"/>
+      <c r="I9" s="48"/>
+      <c r="J9" s="48"/>
+      <c r="K9" s="48"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E10" s="43" t="s">
+      <c r="E10" s="48" t="s">
         <v>54</v>
       </c>
-      <c r="F10" s="43"/>
-      <c r="G10" s="43"/>
-      <c r="H10" s="43"/>
-      <c r="I10" s="43"/>
-      <c r="J10" s="43"/>
-      <c r="K10" s="43"/>
+      <c r="F10" s="48"/>
+      <c r="G10" s="48"/>
+      <c r="H10" s="48"/>
+      <c r="I10" s="48"/>
+      <c r="J10" s="48"/>
+      <c r="K10" s="48"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E11" s="43" t="s">
+      <c r="E11" s="48" t="s">
         <v>55</v>
       </c>
-      <c r="F11" s="43"/>
-      <c r="G11" s="43"/>
-      <c r="H11" s="43"/>
-      <c r="I11" s="43"/>
-      <c r="J11" s="43"/>
-      <c r="K11" s="43"/>
+      <c r="F11" s="48"/>
+      <c r="G11" s="48"/>
+      <c r="H11" s="48"/>
+      <c r="I11" s="48"/>
+      <c r="J11" s="48"/>
+      <c r="K11" s="48"/>
     </row>
     <row r="12" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B12" s="15" t="s">
@@ -1878,45 +2291,45 @@
       </c>
       <c r="C12" s="15"/>
       <c r="D12" s="15"/>
-      <c r="E12" s="43" t="s">
+      <c r="E12" s="48" t="s">
         <v>57</v>
       </c>
-      <c r="F12" s="43"/>
-      <c r="G12" s="43"/>
-      <c r="H12" s="43"/>
-      <c r="I12" s="43"/>
-      <c r="J12" s="43"/>
-      <c r="K12" s="43"/>
-      <c r="L12" s="43"/>
-      <c r="M12" s="43"/>
+      <c r="F12" s="48"/>
+      <c r="G12" s="48"/>
+      <c r="H12" s="48"/>
+      <c r="I12" s="48"/>
+      <c r="J12" s="48"/>
+      <c r="K12" s="48"/>
+      <c r="L12" s="48"/>
+      <c r="M12" s="48"/>
     </row>
     <row r="13" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="16"/>
-      <c r="E13" s="43" t="s">
+      <c r="E13" s="48" t="s">
         <v>58</v>
       </c>
-      <c r="F13" s="43"/>
-      <c r="G13" s="43"/>
-      <c r="H13" s="43"/>
-      <c r="I13" s="43"/>
-      <c r="J13" s="43"/>
-      <c r="K13" s="43"/>
-      <c r="L13" s="43"/>
-      <c r="M13" s="43"/>
+      <c r="F13" s="48"/>
+      <c r="G13" s="48"/>
+      <c r="H13" s="48"/>
+      <c r="I13" s="48"/>
+      <c r="J13" s="48"/>
+      <c r="K13" s="48"/>
+      <c r="L13" s="48"/>
+      <c r="M13" s="48"/>
     </row>
     <row r="14" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="15"/>
-      <c r="E14" s="43" t="s">
+      <c r="E14" s="48" t="s">
         <v>59</v>
       </c>
-      <c r="F14" s="43"/>
-      <c r="G14" s="43"/>
-      <c r="H14" s="43"/>
-      <c r="I14" s="43"/>
-      <c r="J14" s="43"/>
-      <c r="K14" s="43"/>
-      <c r="L14" s="43"/>
-      <c r="M14" s="43"/>
+      <c r="F14" s="48"/>
+      <c r="G14" s="48"/>
+      <c r="H14" s="48"/>
+      <c r="I14" s="48"/>
+      <c r="J14" s="48"/>
+      <c r="K14" s="48"/>
+      <c r="L14" s="48"/>
+      <c r="M14" s="48"/>
     </row>
     <row r="15" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="15"/>
@@ -1944,43 +2357,43 @@
       </c>
       <c r="C17" s="15"/>
       <c r="D17" s="15"/>
-      <c r="E17" s="43" t="s">
+      <c r="E17" s="48" t="s">
         <v>57</v>
       </c>
-      <c r="F17" s="43"/>
-      <c r="G17" s="43"/>
-      <c r="H17" s="43"/>
-      <c r="I17" s="43"/>
-      <c r="J17" s="43"/>
-      <c r="K17" s="43"/>
-      <c r="L17" s="43"/>
-      <c r="M17" s="43"/>
+      <c r="F17" s="48"/>
+      <c r="G17" s="48"/>
+      <c r="H17" s="48"/>
+      <c r="I17" s="48"/>
+      <c r="J17" s="48"/>
+      <c r="K17" s="48"/>
+      <c r="L17" s="48"/>
+      <c r="M17" s="48"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E18" s="43" t="s">
+      <c r="E18" s="48" t="s">
         <v>58</v>
       </c>
-      <c r="F18" s="43"/>
-      <c r="G18" s="43"/>
-      <c r="H18" s="43"/>
-      <c r="I18" s="43"/>
-      <c r="J18" s="43"/>
-      <c r="K18" s="43"/>
-      <c r="L18" s="43"/>
-      <c r="M18" s="43"/>
+      <c r="F18" s="48"/>
+      <c r="G18" s="48"/>
+      <c r="H18" s="48"/>
+      <c r="I18" s="48"/>
+      <c r="J18" s="48"/>
+      <c r="K18" s="48"/>
+      <c r="L18" s="48"/>
+      <c r="M18" s="48"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E19" s="43" t="s">
+      <c r="E19" s="48" t="s">
         <v>59</v>
       </c>
-      <c r="F19" s="43"/>
-      <c r="G19" s="43"/>
-      <c r="H19" s="43"/>
-      <c r="I19" s="43"/>
-      <c r="J19" s="43"/>
-      <c r="K19" s="43"/>
-      <c r="L19" s="43"/>
-      <c r="M19" s="43"/>
+      <c r="F19" s="48"/>
+      <c r="G19" s="48"/>
+      <c r="H19" s="48"/>
+      <c r="I19" s="48"/>
+      <c r="J19" s="48"/>
+      <c r="K19" s="48"/>
+      <c r="L19" s="48"/>
+      <c r="M19" s="48"/>
     </row>
     <row r="20" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="15"/>
@@ -1989,10 +2402,10 @@
       </c>
       <c r="C20" s="15"/>
       <c r="D20" s="15"/>
-      <c r="E20" s="43" t="s">
+      <c r="E20" s="48" t="s">
         <v>60</v>
       </c>
-      <c r="F20" s="43"/>
+      <c r="F20" s="48"/>
     </row>
     <row r="21" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="15"/>
@@ -2020,10 +2433,10 @@
       </c>
       <c r="C23" s="15"/>
       <c r="D23" s="15"/>
-      <c r="E23" s="43" t="s">
+      <c r="E23" s="48" t="s">
         <v>60</v>
       </c>
-      <c r="F23" s="43"/>
+      <c r="F23" s="48"/>
     </row>
     <row r="24" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="5"/>
@@ -2047,8 +2460,360 @@
         <v>32</v>
       </c>
     </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27" s="56" t="s">
+        <v>71</v>
+      </c>
+      <c r="B27" s="56"/>
+      <c r="C27" s="56"/>
+      <c r="D27" s="56"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28" s="57" t="s">
+        <v>72</v>
+      </c>
+      <c r="B28" s="57"/>
+      <c r="C28" s="57"/>
+      <c r="D28" s="57"/>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A29" s="58">
+        <v>41796</v>
+      </c>
+      <c r="B29" s="59"/>
+      <c r="C29" s="60"/>
+      <c r="D29" s="60"/>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A30" s="60"/>
+      <c r="B30" s="60" t="s">
+        <v>25</v>
+      </c>
+      <c r="C30" s="60"/>
+      <c r="D30" s="60"/>
+      <c r="E30" s="48" t="s">
+        <v>82</v>
+      </c>
+      <c r="F30" s="48"/>
+      <c r="G30" s="48"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E31" s="48" t="s">
+        <v>51</v>
+      </c>
+      <c r="F31" s="48"/>
+      <c r="G31" s="48"/>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A32" s="60"/>
+      <c r="B32" s="60" t="s">
+        <v>24</v>
+      </c>
+      <c r="C32" s="60"/>
+      <c r="D32" s="60"/>
+      <c r="E32" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33" s="58">
+        <v>41797</v>
+      </c>
+      <c r="B33" s="60"/>
+      <c r="C33" s="60"/>
+      <c r="D33" s="60"/>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34" s="64"/>
+      <c r="B34" s="64" t="s">
+        <v>28</v>
+      </c>
+      <c r="C34" s="60"/>
+      <c r="D34" s="60"/>
+      <c r="E34" s="48" t="s">
+        <v>82</v>
+      </c>
+      <c r="F34" s="48"/>
+      <c r="G34" s="48"/>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E35" s="48" t="s">
+        <v>51</v>
+      </c>
+      <c r="F35" s="48"/>
+      <c r="G35" s="48"/>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36" s="60"/>
+      <c r="B36" s="60" t="s">
+        <v>29</v>
+      </c>
+      <c r="C36" s="60"/>
+      <c r="D36" s="60"/>
+      <c r="E36" s="48" t="s">
+        <v>84</v>
+      </c>
+      <c r="F36" s="48"/>
+      <c r="G36" s="48"/>
+      <c r="H36" s="48"/>
+      <c r="I36" s="48"/>
+      <c r="J36" s="48"/>
+      <c r="K36" s="48"/>
+      <c r="L36" s="48"/>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E37" s="48" t="s">
+        <v>85</v>
+      </c>
+      <c r="F37" s="48"/>
+      <c r="G37" s="48"/>
+      <c r="H37" s="48"/>
+      <c r="I37" s="48"/>
+      <c r="J37" s="48"/>
+      <c r="K37" s="48"/>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E38" s="48" t="s">
+        <v>48</v>
+      </c>
+      <c r="F38" s="48"/>
+      <c r="G38" s="48"/>
+      <c r="H38" s="48"/>
+      <c r="I38" s="48"/>
+      <c r="J38" s="48"/>
+      <c r="K38" s="48"/>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E39" s="48" t="s">
+        <v>86</v>
+      </c>
+      <c r="F39" s="48"/>
+      <c r="G39" s="48"/>
+      <c r="H39" s="48"/>
+      <c r="I39" s="48"/>
+      <c r="J39" s="48"/>
+      <c r="K39" s="48"/>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A40" s="60"/>
+      <c r="B40" s="60" t="s">
+        <v>30</v>
+      </c>
+      <c r="C40" s="60"/>
+      <c r="D40" s="60"/>
+      <c r="E40" s="48" t="s">
+        <v>87</v>
+      </c>
+      <c r="F40" s="48"/>
+      <c r="G40" s="48"/>
+      <c r="H40" s="48"/>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A41" s="58">
+        <v>41798</v>
+      </c>
+      <c r="B41" s="60"/>
+      <c r="C41" s="60"/>
+      <c r="D41" s="60"/>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A42" s="64"/>
+      <c r="B42" s="64" t="s">
+        <v>28</v>
+      </c>
+      <c r="C42" s="60"/>
+      <c r="D42" s="60"/>
+      <c r="E42" s="48" t="s">
+        <v>84</v>
+      </c>
+      <c r="F42" s="48"/>
+      <c r="G42" s="48"/>
+      <c r="H42" s="48"/>
+      <c r="I42" s="48"/>
+      <c r="J42" s="48"/>
+      <c r="K42" s="48"/>
+      <c r="L42" s="48"/>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E43" s="48" t="s">
+        <v>85</v>
+      </c>
+      <c r="F43" s="48"/>
+      <c r="G43" s="48"/>
+      <c r="H43" s="48"/>
+      <c r="I43" s="48"/>
+      <c r="J43" s="48"/>
+      <c r="K43" s="48"/>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E44" s="48" t="s">
+        <v>48</v>
+      </c>
+      <c r="F44" s="48"/>
+      <c r="G44" s="48"/>
+      <c r="H44" s="48"/>
+      <c r="I44" s="48"/>
+      <c r="J44" s="48"/>
+      <c r="K44" s="48"/>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E45" s="48" t="s">
+        <v>86</v>
+      </c>
+      <c r="F45" s="48"/>
+      <c r="G45" s="48"/>
+      <c r="H45" s="48"/>
+      <c r="I45" s="48"/>
+      <c r="J45" s="48"/>
+      <c r="K45" s="48"/>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A46" s="60"/>
+      <c r="B46" s="60" t="s">
+        <v>29</v>
+      </c>
+      <c r="C46" s="60"/>
+      <c r="D46" s="60"/>
+      <c r="E46" s="48" t="s">
+        <v>62</v>
+      </c>
+      <c r="F46" s="48"/>
+      <c r="G46" s="48"/>
+      <c r="H46" s="48"/>
+      <c r="I46" s="48"/>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E47" s="48" t="s">
+        <v>88</v>
+      </c>
+      <c r="F47" s="48"/>
+      <c r="G47" s="48"/>
+      <c r="H47" s="48"/>
+      <c r="I47" s="48"/>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A48" s="60"/>
+      <c r="B48" s="60" t="s">
+        <v>30</v>
+      </c>
+      <c r="C48" s="60"/>
+      <c r="D48" s="60"/>
+      <c r="E48" s="48" t="s">
+        <v>87</v>
+      </c>
+      <c r="F48" s="48"/>
+      <c r="G48" s="48"/>
+      <c r="H48" s="48"/>
+      <c r="I48" s="48"/>
+      <c r="J48" s="48"/>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A49" s="62">
+        <v>41800</v>
+      </c>
+      <c r="B49" s="59"/>
+      <c r="C49" s="59"/>
+      <c r="D49" s="59"/>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A50" s="59"/>
+      <c r="B50" s="64" t="s">
+        <v>28</v>
+      </c>
+      <c r="C50" s="60"/>
+      <c r="D50" s="60"/>
+      <c r="E50" s="48" t="s">
+        <v>62</v>
+      </c>
+      <c r="F50" s="48"/>
+      <c r="G50" s="48"/>
+      <c r="H50" s="48"/>
+      <c r="I50" s="48"/>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E51" s="48" t="s">
+        <v>88</v>
+      </c>
+      <c r="F51" s="48"/>
+      <c r="G51" s="48"/>
+      <c r="H51" s="48"/>
+      <c r="I51" s="48"/>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A52" s="59"/>
+      <c r="B52" s="60" t="s">
+        <v>29</v>
+      </c>
+      <c r="C52" s="60"/>
+      <c r="D52" s="60"/>
+      <c r="E52" s="48" t="s">
+        <v>62</v>
+      </c>
+      <c r="F52" s="48"/>
+      <c r="G52" s="48"/>
+      <c r="H52" s="48"/>
+      <c r="I52" s="48"/>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E53" s="48" t="s">
+        <v>88</v>
+      </c>
+      <c r="F53" s="48"/>
+      <c r="G53" s="48"/>
+      <c r="H53" s="48"/>
+      <c r="I53" s="48"/>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A54" s="59"/>
+      <c r="B54" s="60" t="s">
+        <v>30</v>
+      </c>
+      <c r="C54" s="60"/>
+      <c r="D54" s="60"/>
+      <c r="E54" s="48" t="s">
+        <v>87</v>
+      </c>
+      <c r="F54" s="48"/>
+      <c r="G54" s="48"/>
+      <c r="H54" s="48"/>
+      <c r="I54" s="48"/>
+      <c r="J54" s="48"/>
+    </row>
   </sheetData>
-  <mergeCells count="19">
+  <mergeCells count="42">
+    <mergeCell ref="E52:I52"/>
+    <mergeCell ref="E53:I53"/>
+    <mergeCell ref="E54:J54"/>
+    <mergeCell ref="E46:I46"/>
+    <mergeCell ref="E47:I47"/>
+    <mergeCell ref="E48:J48"/>
+    <mergeCell ref="E50:I50"/>
+    <mergeCell ref="E51:I51"/>
+    <mergeCell ref="E40:H40"/>
+    <mergeCell ref="E42:L42"/>
+    <mergeCell ref="E43:K43"/>
+    <mergeCell ref="E44:K44"/>
+    <mergeCell ref="E45:K45"/>
+    <mergeCell ref="E35:G35"/>
+    <mergeCell ref="E36:L36"/>
+    <mergeCell ref="E37:K37"/>
+    <mergeCell ref="E38:K38"/>
+    <mergeCell ref="E39:K39"/>
+    <mergeCell ref="A27:D27"/>
+    <mergeCell ref="A28:D28"/>
+    <mergeCell ref="E30:G30"/>
+    <mergeCell ref="E31:G31"/>
+    <mergeCell ref="E34:G34"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="E4:K4"/>
+    <mergeCell ref="E5:K5"/>
+    <mergeCell ref="E6:K6"/>
+    <mergeCell ref="E7:J7"/>
+    <mergeCell ref="E9:K9"/>
+    <mergeCell ref="E10:K10"/>
+    <mergeCell ref="E11:K11"/>
     <mergeCell ref="B7:D7"/>
     <mergeCell ref="E23:F23"/>
     <mergeCell ref="E19:M19"/>
@@ -2058,16 +2823,6 @@
     <mergeCell ref="E14:M14"/>
     <mergeCell ref="E17:M17"/>
     <mergeCell ref="E18:M18"/>
-    <mergeCell ref="E6:K6"/>
-    <mergeCell ref="E7:J7"/>
-    <mergeCell ref="E9:K9"/>
-    <mergeCell ref="E10:K10"/>
-    <mergeCell ref="E11:K11"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="E4:K4"/>
-    <mergeCell ref="E5:K5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2075,32 +2830,32 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O31"/>
+  <dimension ref="A1:O56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="A32" sqref="A32:L56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="42" t="s">
+      <c r="A2" s="44" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="42"/>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
+      <c r="B2" s="44"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
     </row>
     <row r="3" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="50">
+      <c r="A3" s="20">
         <v>41792</v>
       </c>
       <c r="B3" s="5"/>
@@ -2109,18 +2864,18 @@
     </row>
     <row r="4" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="17"/>
-      <c r="B4" s="41" t="s">
+      <c r="B4" s="46" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="41"/>
-      <c r="D4" s="41"/>
-      <c r="E4" s="54" t="s">
+      <c r="C4" s="46"/>
+      <c r="D4" s="46"/>
+      <c r="E4" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="F4" s="54"/>
-      <c r="G4" s="54"/>
-      <c r="H4" s="54"/>
-      <c r="I4" s="54"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="23"/>
+      <c r="I4" s="23"/>
     </row>
     <row r="5" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="17"/>
@@ -2133,23 +2888,23 @@
     </row>
     <row r="6" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="17"/>
-      <c r="B6" s="41" t="s">
+      <c r="B6" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="41"/>
-      <c r="D6" s="41"/>
+      <c r="C6" s="46"/>
+      <c r="D6" s="46"/>
       <c r="E6" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="17"/>
-      <c r="B7" s="41"/>
-      <c r="C7" s="41"/>
-      <c r="D7" s="41"/>
+      <c r="B7" s="46"/>
+      <c r="C7" s="46"/>
+      <c r="D7" s="46"/>
     </row>
     <row r="8" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="51">
+      <c r="A8" s="21">
         <v>41793</v>
       </c>
       <c r="B8" s="18"/>
@@ -2163,17 +2918,17 @@
       </c>
       <c r="C9" s="18"/>
       <c r="D9" s="18"/>
-      <c r="E9" s="43" t="s">
+      <c r="E9" s="48" t="s">
         <v>64</v>
       </c>
-      <c r="F9" s="43"/>
-      <c r="G9" s="43"/>
-      <c r="H9" s="43"/>
-      <c r="I9" s="43"/>
-      <c r="J9" s="43"/>
-      <c r="K9" s="43"/>
-      <c r="L9" s="43"/>
-      <c r="M9" s="43"/>
+      <c r="F9" s="48"/>
+      <c r="G9" s="48"/>
+      <c r="H9" s="48"/>
+      <c r="I9" s="48"/>
+      <c r="J9" s="48"/>
+      <c r="K9" s="48"/>
+      <c r="L9" s="48"/>
+      <c r="M9" s="48"/>
     </row>
     <row r="10" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="17"/>
@@ -2186,17 +2941,17 @@
     </row>
     <row r="11" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="17"/>
-      <c r="B11" s="41"/>
-      <c r="C11" s="41"/>
-      <c r="D11" s="41"/>
+      <c r="B11" s="46"/>
+      <c r="C11" s="46"/>
+      <c r="D11" s="46"/>
     </row>
     <row r="12" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="17"/>
-      <c r="B12" s="41" t="s">
+      <c r="B12" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="41"/>
-      <c r="D12" s="41"/>
+      <c r="C12" s="46"/>
+      <c r="D12" s="46"/>
       <c r="E12" t="s">
         <v>65</v>
       </c>
@@ -2206,16 +2961,16 @@
       <c r="B13" s="18"/>
       <c r="C13" s="18"/>
       <c r="D13" s="18"/>
-      <c r="E13" s="43" t="s">
+      <c r="E13" s="48" t="s">
         <v>66</v>
       </c>
-      <c r="F13" s="43"/>
-      <c r="G13" s="43"/>
-      <c r="H13" s="43"/>
-      <c r="I13" s="43"/>
-      <c r="J13" s="43"/>
-      <c r="K13" s="43"/>
-      <c r="L13" s="43"/>
+      <c r="F13" s="48"/>
+      <c r="G13" s="48"/>
+      <c r="H13" s="48"/>
+      <c r="I13" s="48"/>
+      <c r="J13" s="48"/>
+      <c r="K13" s="48"/>
+      <c r="L13" s="48"/>
     </row>
     <row r="14" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="17"/>
@@ -2225,14 +2980,14 @@
     </row>
     <row r="15" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="17"/>
-      <c r="B15" s="41" t="s">
+      <c r="B15" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="C15" s="41"/>
-      <c r="D15" s="41"/>
+      <c r="C15" s="46"/>
+      <c r="D15" s="46"/>
     </row>
     <row r="16" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="51">
+      <c r="A16" s="21">
         <v>41794</v>
       </c>
       <c r="B16" s="18"/>
@@ -2241,45 +2996,45 @@
     </row>
     <row r="17" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="17"/>
-      <c r="B17" s="39" t="s">
+      <c r="B17" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="C17" s="39"/>
-      <c r="D17" s="39"/>
-      <c r="E17" s="43" t="s">
+      <c r="C17" s="45"/>
+      <c r="D17" s="45"/>
+      <c r="E17" s="48" t="s">
         <v>67</v>
       </c>
-      <c r="F17" s="43"/>
-      <c r="G17" s="43"/>
-      <c r="H17" s="43"/>
-      <c r="I17" s="43"/>
-      <c r="J17" s="43"/>
-      <c r="K17" s="43"/>
+      <c r="F17" s="48"/>
+      <c r="G17" s="48"/>
+      <c r="H17" s="48"/>
+      <c r="I17" s="48"/>
+      <c r="J17" s="48"/>
+      <c r="K17" s="48"/>
     </row>
     <row r="18" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="17"/>
       <c r="B18" s="18"/>
       <c r="C18" s="18"/>
       <c r="D18" s="18"/>
-      <c r="E18" s="43" t="s">
+      <c r="E18" s="48" t="s">
         <v>68</v>
       </c>
-      <c r="F18" s="43"/>
-      <c r="G18" s="43"/>
-      <c r="H18" s="43"/>
-      <c r="I18" s="43"/>
-      <c r="J18" s="43"/>
-      <c r="K18" s="43"/>
+      <c r="F18" s="48"/>
+      <c r="G18" s="48"/>
+      <c r="H18" s="48"/>
+      <c r="I18" s="48"/>
+      <c r="J18" s="48"/>
+      <c r="K18" s="48"/>
     </row>
     <row r="19" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="17"/>
       <c r="B19" s="18"/>
       <c r="C19" s="18"/>
       <c r="D19" s="18"/>
-      <c r="E19" s="43" t="s">
+      <c r="E19" s="48" t="s">
         <v>41</v>
       </c>
-      <c r="F19" s="43"/>
+      <c r="F19" s="48"/>
     </row>
     <row r="20" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="17"/>
@@ -2289,45 +3044,45 @@
     </row>
     <row r="21" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="17"/>
-      <c r="B21" s="41" t="s">
+      <c r="B21" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="C21" s="41"/>
-      <c r="D21" s="41"/>
-      <c r="E21" s="43" t="s">
+      <c r="C21" s="46"/>
+      <c r="D21" s="46"/>
+      <c r="E21" s="48" t="s">
         <v>45</v>
       </c>
-      <c r="F21" s="43"/>
-      <c r="G21" s="43"/>
-      <c r="H21" s="43"/>
-      <c r="I21" s="43"/>
-      <c r="J21" s="43"/>
-      <c r="K21" s="43"/>
-      <c r="L21" s="43"/>
-      <c r="M21" s="43"/>
-      <c r="N21" s="43"/>
-      <c r="O21" s="43"/>
+      <c r="F21" s="48"/>
+      <c r="G21" s="48"/>
+      <c r="H21" s="48"/>
+      <c r="I21" s="48"/>
+      <c r="J21" s="48"/>
+      <c r="K21" s="48"/>
+      <c r="L21" s="48"/>
+      <c r="M21" s="48"/>
+      <c r="N21" s="48"/>
+      <c r="O21" s="48"/>
     </row>
     <row r="22" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="17"/>
       <c r="B22" s="18"/>
       <c r="C22" s="18"/>
       <c r="D22" s="18"/>
-      <c r="E22" s="43" t="s">
+      <c r="E22" s="48" t="s">
         <v>69</v>
       </c>
-      <c r="F22" s="43"/>
+      <c r="F22" s="48"/>
     </row>
     <row r="23" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="17"/>
-      <c r="B23" s="41" t="s">
+      <c r="B23" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="C23" s="41"/>
-      <c r="D23" s="41"/>
+      <c r="C23" s="46"/>
+      <c r="D23" s="46"/>
     </row>
     <row r="24" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="52">
+      <c r="A24" s="22">
         <v>41795</v>
       </c>
       <c r="B24" s="10"/>
@@ -2362,47 +3117,348 @@
     </row>
     <row r="28" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="5"/>
-      <c r="B28" s="41" t="s">
+      <c r="B28" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="C28" s="41"/>
-      <c r="D28" s="41"/>
-      <c r="E28" s="43" t="s">
+      <c r="C28" s="46"/>
+      <c r="D28" s="46"/>
+      <c r="E28" s="48" t="s">
         <v>62</v>
       </c>
-      <c r="F28" s="43"/>
-      <c r="G28" s="43"/>
-      <c r="H28" s="43"/>
+      <c r="F28" s="48"/>
+      <c r="G28" s="48"/>
+      <c r="H28" s="48"/>
     </row>
     <row r="29" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="5"/>
       <c r="B29" s="18"/>
       <c r="C29" s="18"/>
       <c r="D29" s="18"/>
-      <c r="E29" s="43"/>
-      <c r="F29" s="43"/>
+      <c r="E29" s="48"/>
+      <c r="F29" s="48"/>
     </row>
     <row r="30" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="5"/>
-      <c r="B30" s="39" t="s">
+      <c r="B30" s="45" t="s">
         <v>30</v>
       </c>
-      <c r="C30" s="39"/>
-      <c r="D30" s="39"/>
-      <c r="E30" s="53" t="s">
+      <c r="C30" s="45"/>
+      <c r="D30" s="45"/>
+      <c r="E30" s="55" t="s">
         <v>70</v>
       </c>
-      <c r="F30" s="53"/>
-      <c r="G30" s="53"/>
+      <c r="F30" s="55"/>
+      <c r="G30" s="55"/>
     </row>
     <row r="31" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="5"/>
-      <c r="B31" s="39"/>
-      <c r="C31" s="39"/>
-      <c r="D31" s="39"/>
+      <c r="B31" s="45"/>
+      <c r="C31" s="45"/>
+      <c r="D31" s="45"/>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A32" s="56" t="s">
+        <v>71</v>
+      </c>
+      <c r="B32" s="56"/>
+      <c r="C32" s="56"/>
+      <c r="D32" s="56"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="57" t="s">
+        <v>72</v>
+      </c>
+      <c r="B33" s="57"/>
+      <c r="C33" s="57"/>
+      <c r="D33" s="57"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="65">
+        <v>41796</v>
+      </c>
+      <c r="B34" s="59"/>
+      <c r="C34" s="60"/>
+      <c r="D34" s="60"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="60"/>
+      <c r="B35" s="61" t="s">
+        <v>25</v>
+      </c>
+      <c r="C35" s="61"/>
+      <c r="D35" s="61"/>
+      <c r="E35" s="48" t="s">
+        <v>89</v>
+      </c>
+      <c r="F35" s="48"/>
+      <c r="G35" s="48"/>
+      <c r="H35" s="48"/>
+      <c r="I35" s="48"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="66"/>
+      <c r="B36" s="61"/>
+      <c r="C36" s="61"/>
+      <c r="D36" s="61"/>
+      <c r="E36" s="48" t="s">
+        <v>51</v>
+      </c>
+      <c r="F36" s="48"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="67"/>
+      <c r="B37" s="61" t="s">
+        <v>24</v>
+      </c>
+      <c r="C37" s="61"/>
+      <c r="D37" s="61"/>
+      <c r="E37" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="65">
+        <v>41797</v>
+      </c>
+      <c r="F38" s="23"/>
+      <c r="G38" s="23"/>
+      <c r="H38" s="23"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" s="68"/>
+      <c r="B39" s="64" t="s">
+        <v>28</v>
+      </c>
+      <c r="C39" s="60"/>
+      <c r="D39" s="60"/>
+      <c r="E39" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="F39" s="23"/>
+      <c r="G39" s="23"/>
+      <c r="H39" s="23"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="60"/>
+      <c r="B40" s="61"/>
+      <c r="C40" s="61"/>
+      <c r="D40" s="61"/>
+      <c r="E40" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="F40" s="23"/>
+      <c r="G40" s="23"/>
+      <c r="H40" s="23"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" s="69"/>
+      <c r="B41" s="61" t="s">
+        <v>29</v>
+      </c>
+      <c r="C41" s="61"/>
+      <c r="D41" s="61"/>
+      <c r="E41" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" s="69"/>
+      <c r="B42" s="60"/>
+      <c r="C42" s="60"/>
+      <c r="D42" s="60"/>
+      <c r="E42" s="23" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" s="70"/>
+      <c r="B43" s="61" t="s">
+        <v>30</v>
+      </c>
+      <c r="C43" s="61"/>
+      <c r="D43" s="61"/>
+      <c r="E43" s="23" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" s="65">
+        <v>41798</v>
+      </c>
+      <c r="C44" s="60"/>
+      <c r="D44" s="60"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" s="70"/>
+      <c r="B45" s="64" t="s">
+        <v>28</v>
+      </c>
+      <c r="C45" s="60"/>
+      <c r="D45" s="60"/>
+      <c r="E45" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" s="70"/>
+      <c r="B46" s="64"/>
+      <c r="C46" s="60"/>
+      <c r="D46" s="60"/>
+      <c r="E46" s="23" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" s="60"/>
+      <c r="B47" s="61" t="s">
+        <v>29</v>
+      </c>
+      <c r="C47" s="61"/>
+      <c r="D47" s="61"/>
+      <c r="E47" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" s="60"/>
+      <c r="B48" s="60"/>
+      <c r="C48" s="60"/>
+      <c r="D48" s="60"/>
+      <c r="E48" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A49" s="60"/>
+      <c r="B49" s="61" t="s">
+        <v>30</v>
+      </c>
+      <c r="C49" s="61"/>
+      <c r="D49" s="61"/>
+      <c r="E49" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A50" s="71">
+        <v>41800</v>
+      </c>
+      <c r="B50" s="59"/>
+      <c r="C50" s="59"/>
+      <c r="D50" s="59"/>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A51" s="59"/>
+      <c r="B51" s="64" t="s">
+        <v>28</v>
+      </c>
+      <c r="C51" s="60"/>
+      <c r="D51" s="60"/>
+      <c r="E51" t="s">
+        <v>77</v>
+      </c>
+      <c r="F51" s="23"/>
+      <c r="G51" s="23"/>
+      <c r="H51" s="23"/>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A52" s="59"/>
+      <c r="B52" s="64"/>
+      <c r="C52" s="60"/>
+      <c r="D52" s="60"/>
+      <c r="E52" t="s">
+        <v>51</v>
+      </c>
+      <c r="F52" s="23"/>
+      <c r="G52" s="23"/>
+      <c r="H52" s="23"/>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A53" s="59"/>
+      <c r="B53" s="61" t="s">
+        <v>29</v>
+      </c>
+      <c r="C53" s="61"/>
+      <c r="D53" s="61"/>
+      <c r="E53" s="23" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A54" s="59"/>
+      <c r="B54" s="60"/>
+      <c r="C54" s="60"/>
+      <c r="D54" s="60"/>
+      <c r="E54" s="48" t="s">
+        <v>94</v>
+      </c>
+      <c r="F54" s="48"/>
+      <c r="G54" s="48"/>
+      <c r="H54" s="48"/>
+      <c r="I54" s="48"/>
+      <c r="J54" s="48"/>
+      <c r="K54" s="48"/>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A55" s="59"/>
+      <c r="B55" s="60"/>
+      <c r="C55" s="60"/>
+      <c r="D55" s="60"/>
+      <c r="E55" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="F55" s="19"/>
+      <c r="G55" s="19"/>
+      <c r="H55" s="19"/>
+      <c r="I55" s="19"/>
+      <c r="J55" s="19"/>
+      <c r="K55" s="19"/>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A56" s="59"/>
+      <c r="B56" s="61" t="s">
+        <v>30</v>
+      </c>
+      <c r="C56" s="61"/>
+      <c r="D56" s="61"/>
+      <c r="E56" s="23" t="s">
+        <v>92</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="24">
+  <mergeCells count="39">
+    <mergeCell ref="B56:D56"/>
+    <mergeCell ref="A33:D33"/>
+    <mergeCell ref="E35:I35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="B41:D41"/>
+    <mergeCell ref="B43:D43"/>
+    <mergeCell ref="B47:D47"/>
+    <mergeCell ref="B49:D49"/>
+    <mergeCell ref="B53:D53"/>
+    <mergeCell ref="E54:K54"/>
+    <mergeCell ref="B40:D40"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A32:D32"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="E9:M9"/>
+    <mergeCell ref="E13:L13"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="E17:K17"/>
+    <mergeCell ref="E18:K18"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="E21:O21"/>
+    <mergeCell ref="E22:F22"/>
     <mergeCell ref="B31:D31"/>
     <mergeCell ref="B23:D23"/>
     <mergeCell ref="B28:D28"/>
@@ -2410,23 +3466,6 @@
     <mergeCell ref="E29:F29"/>
     <mergeCell ref="B30:D30"/>
     <mergeCell ref="E30:G30"/>
-    <mergeCell ref="E18:K18"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="E21:O21"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="E9:M9"/>
-    <mergeCell ref="E13:L13"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="E17:K17"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A1:D1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Memperbaharui informasi logbook team(13juni2014)
</commit_message>
<xml_diff>
--- a/src/log-book/LogBook-speaker-team.xlsx
+++ b/src/log-book/LogBook-speaker-team.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Informasi Umum" sheetId="1" r:id="rId1"/>
@@ -13,7 +13,7 @@
     <sheet name="DAILY SCRUM-Leni" sheetId="4" r:id="rId4"/>
     <sheet name="DAILY SCRUM-Hayati" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="112">
   <si>
     <t>Nama kelompok</t>
   </si>
@@ -350,6 +350,15 @@
   </si>
   <si>
     <t>Merging</t>
+  </si>
+  <si>
+    <t>Mengedit style css untuk cover slide bespoke (lanjutan)</t>
+  </si>
+  <si>
+    <t>Perbaharui kesalahan-kesalahan kosakata di slide.</t>
+  </si>
+  <si>
+    <t>Memperbaharui informasi logbook tem</t>
   </si>
 </sst>
 </file>
@@ -629,7 +638,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -735,6 +744,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -750,33 +784,12 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -795,27 +808,27 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -845,9 +858,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1121,7 +1131,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1143,99 +1153,99 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="33" x14ac:dyDescent="0.25">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-      <c r="I1" s="39"/>
-      <c r="J1" s="39"/>
-      <c r="K1" s="39"/>
-      <c r="L1" s="39"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
+      <c r="I1" s="48"/>
+      <c r="J1" s="48"/>
+      <c r="K1" s="48"/>
+      <c r="L1" s="48"/>
     </row>
     <row r="2" spans="1:12" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A2" s="47" t="s">
+      <c r="A2" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="47"/>
-      <c r="C2" s="47"/>
-      <c r="D2" s="40" t="s">
+      <c r="B2" s="53"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
-      <c r="J2" s="40"/>
-      <c r="K2" s="40"/>
-      <c r="L2" s="40"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="49"/>
+      <c r="K2" s="49"/>
+      <c r="L2" s="49"/>
     </row>
     <row r="3" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="47" t="s">
+      <c r="A3" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="47"/>
-      <c r="C3" s="47"/>
-      <c r="D3" s="48" t="s">
+      <c r="B3" s="53"/>
+      <c r="C3" s="53"/>
+      <c r="D3" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="48"/>
-      <c r="F3" s="48"/>
-      <c r="G3" s="48"/>
-      <c r="H3" s="48"/>
-      <c r="I3" s="48"/>
-      <c r="J3" s="48"/>
-      <c r="K3" s="48"/>
-      <c r="L3" s="48"/>
+      <c r="E3" s="54"/>
+      <c r="F3" s="54"/>
+      <c r="G3" s="54"/>
+      <c r="H3" s="54"/>
+      <c r="I3" s="54"/>
+      <c r="J3" s="54"/>
+      <c r="K3" s="54"/>
+      <c r="L3" s="54"/>
     </row>
     <row r="4" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="47" t="s">
+      <c r="A4" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="47"/>
-      <c r="C4" s="47"/>
-      <c r="D4" s="41" t="s">
+      <c r="B4" s="53"/>
+      <c r="C4" s="53"/>
+      <c r="D4" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="41"/>
-      <c r="F4" s="41"/>
-      <c r="G4" s="41"/>
-      <c r="H4" s="41"/>
-      <c r="I4" s="41"/>
-      <c r="J4" s="41"/>
-      <c r="K4" s="41"/>
-      <c r="L4" s="41"/>
+      <c r="E4" s="50"/>
+      <c r="F4" s="50"/>
+      <c r="G4" s="50"/>
+      <c r="H4" s="50"/>
+      <c r="I4" s="50"/>
+      <c r="J4" s="50"/>
+      <c r="K4" s="50"/>
+      <c r="L4" s="50"/>
     </row>
     <row r="5" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="47" t="s">
+      <c r="A5" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="47"/>
-      <c r="C5" s="47"/>
-      <c r="D5" s="41" t="s">
+      <c r="B5" s="53"/>
+      <c r="C5" s="53"/>
+      <c r="D5" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="41"/>
-      <c r="F5" s="41"/>
-      <c r="G5" s="41"/>
-      <c r="H5" s="41"/>
-      <c r="I5" s="41"/>
-      <c r="J5" s="41"/>
-      <c r="K5" s="41"/>
-      <c r="L5" s="41"/>
+      <c r="E5" s="50"/>
+      <c r="F5" s="50"/>
+      <c r="G5" s="50"/>
+      <c r="H5" s="50"/>
+      <c r="I5" s="50"/>
+      <c r="J5" s="50"/>
+      <c r="K5" s="50"/>
+      <c r="L5" s="50"/>
     </row>
     <row r="6" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="42" t="s">
+      <c r="A6" s="51" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="43"/>
-      <c r="C6" s="43"/>
+      <c r="B6" s="52"/>
+      <c r="C6" s="52"/>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
       <c r="F6" s="11"/>
@@ -1244,7 +1254,7 @@
       <c r="I6" s="11"/>
       <c r="J6" s="11"/>
       <c r="K6" s="11"/>
-      <c r="L6" s="52"/>
+      <c r="L6" s="44"/>
     </row>
     <row r="7" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A7" s="12"/>
@@ -1252,17 +1262,17 @@
         <v>6</v>
       </c>
       <c r="C7" s="11"/>
-      <c r="D7" s="46" t="s">
+      <c r="D7" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="46"/>
+      <c r="E7" s="47"/>
       <c r="F7" s="11"/>
       <c r="G7" s="11"/>
       <c r="H7" s="11"/>
       <c r="I7" s="11"/>
       <c r="J7" s="11"/>
       <c r="K7" s="11"/>
-      <c r="L7" s="52"/>
+      <c r="L7" s="44"/>
     </row>
     <row r="8" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A8" s="12"/>
@@ -1270,24 +1280,24 @@
         <v>7</v>
       </c>
       <c r="C8" s="11"/>
-      <c r="D8" s="46">
+      <c r="D8" s="47">
         <v>121112295</v>
       </c>
-      <c r="E8" s="46"/>
+      <c r="E8" s="47"/>
       <c r="F8" s="11"/>
       <c r="G8" s="11"/>
       <c r="H8" s="11"/>
       <c r="I8" s="11"/>
       <c r="J8" s="11"/>
       <c r="K8" s="11"/>
-      <c r="L8" s="52"/>
+      <c r="L8" s="44"/>
     </row>
     <row r="9" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="44" t="s">
+      <c r="A9" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="45"/>
-      <c r="C9" s="45"/>
+      <c r="B9" s="46"/>
+      <c r="C9" s="46"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
       <c r="F9" s="11"/>
@@ -1296,7 +1306,7 @@
       <c r="I9" s="11"/>
       <c r="J9" s="11"/>
       <c r="K9" s="11"/>
-      <c r="L9" s="52"/>
+      <c r="L9" s="44"/>
     </row>
     <row r="10" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A10" s="12"/>
@@ -1304,17 +1314,17 @@
         <v>6</v>
       </c>
       <c r="C10" s="11"/>
-      <c r="D10" s="46" t="s">
+      <c r="D10" s="47" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="46"/>
+      <c r="E10" s="47"/>
       <c r="F10" s="11"/>
       <c r="G10" s="11"/>
       <c r="H10" s="11"/>
       <c r="I10" s="11"/>
       <c r="J10" s="11"/>
       <c r="K10" s="11"/>
-      <c r="L10" s="52"/>
+      <c r="L10" s="44"/>
     </row>
     <row r="11" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A11" s="12"/>
@@ -1322,24 +1332,24 @@
         <v>7</v>
       </c>
       <c r="C11" s="11"/>
-      <c r="D11" s="46">
+      <c r="D11" s="47">
         <v>121112911</v>
       </c>
-      <c r="E11" s="46"/>
+      <c r="E11" s="47"/>
       <c r="F11" s="11"/>
       <c r="G11" s="11"/>
       <c r="H11" s="11"/>
       <c r="I11" s="11"/>
       <c r="J11" s="11"/>
       <c r="K11" s="11"/>
-      <c r="L11" s="52"/>
+      <c r="L11" s="44"/>
     </row>
     <row r="12" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="44" t="s">
+      <c r="A12" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="45"/>
-      <c r="C12" s="45"/>
+      <c r="B12" s="46"/>
+      <c r="C12" s="46"/>
       <c r="D12" s="11"/>
       <c r="E12" s="11"/>
       <c r="F12" s="11"/>
@@ -1348,7 +1358,7 @@
       <c r="I12" s="11"/>
       <c r="J12" s="11"/>
       <c r="K12" s="11"/>
-      <c r="L12" s="52"/>
+      <c r="L12" s="44"/>
     </row>
     <row r="13" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A13" s="11"/>
@@ -1356,17 +1366,17 @@
         <v>6</v>
       </c>
       <c r="C13" s="11"/>
-      <c r="D13" s="46" t="s">
+      <c r="D13" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="E13" s="46"/>
+      <c r="E13" s="47"/>
       <c r="F13" s="11"/>
       <c r="G13" s="11"/>
       <c r="H13" s="11"/>
       <c r="I13" s="11"/>
       <c r="J13" s="11"/>
       <c r="K13" s="11"/>
-      <c r="L13" s="52"/>
+      <c r="L13" s="44"/>
     </row>
     <row r="14" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A14" s="11"/>
@@ -1374,41 +1384,34 @@
         <v>7</v>
       </c>
       <c r="C14" s="11"/>
-      <c r="D14" s="46">
+      <c r="D14" s="47">
         <v>121112724</v>
       </c>
-      <c r="E14" s="46"/>
+      <c r="E14" s="47"/>
       <c r="F14" s="11"/>
       <c r="G14" s="11"/>
       <c r="H14" s="11"/>
       <c r="I14" s="11"/>
       <c r="J14" s="11"/>
       <c r="K14" s="11"/>
-      <c r="L14" s="52"/>
+      <c r="L14" s="44"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="49"/>
-      <c r="B15" s="50"/>
-      <c r="C15" s="50"/>
-      <c r="D15" s="50"/>
-      <c r="E15" s="50"/>
-      <c r="F15" s="50"/>
-      <c r="G15" s="50"/>
-      <c r="H15" s="50"/>
-      <c r="I15" s="50"/>
-      <c r="J15" s="50"/>
-      <c r="K15" s="50"/>
-      <c r="L15" s="51"/>
+      <c r="A15" s="41"/>
+      <c r="B15" s="42"/>
+      <c r="C15" s="42"/>
+      <c r="D15" s="42"/>
+      <c r="E15" s="42"/>
+      <c r="F15" s="42"/>
+      <c r="G15" s="42"/>
+      <c r="H15" s="42"/>
+      <c r="I15" s="42"/>
+      <c r="J15" s="42"/>
+      <c r="K15" s="42"/>
+      <c r="L15" s="43"/>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="A15:L15"/>
-    <mergeCell ref="L6:L14"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D14:E14"/>
     <mergeCell ref="A1:L1"/>
     <mergeCell ref="D2:L2"/>
     <mergeCell ref="D4:L4"/>
@@ -1422,6 +1425,13 @@
     <mergeCell ref="A5:C5"/>
     <mergeCell ref="D5:L5"/>
     <mergeCell ref="D3:L3"/>
+    <mergeCell ref="A15:L15"/>
+    <mergeCell ref="L6:L14"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D14:E14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1445,125 +1455,125 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="58" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="55"/>
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="57"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="58" t="s">
+      <c r="A2" s="60" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="58"/>
-      <c r="C2" s="58"/>
+      <c r="B2" s="60"/>
+      <c r="C2" s="60"/>
       <c r="D2" s="3"/>
-      <c r="E2" s="55"/>
+      <c r="E2" s="57"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="57" t="s">
+      <c r="A3" s="59" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="57"/>
-      <c r="C3" s="57"/>
-      <c r="D3" s="57"/>
-      <c r="E3" s="55"/>
+      <c r="B3" s="59"/>
+      <c r="C3" s="59"/>
+      <c r="D3" s="59"/>
+      <c r="E3" s="57"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="57" t="s">
+      <c r="A4" s="59" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="57"/>
+      <c r="B4" s="59"/>
       <c r="C4" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D4" s="3">
         <v>121112295</v>
       </c>
-      <c r="E4" s="55"/>
+      <c r="E4" s="57"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="58" t="s">
+      <c r="A5" s="60" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="58"/>
-      <c r="C5" s="58"/>
+      <c r="B5" s="60"/>
+      <c r="C5" s="60"/>
       <c r="D5" s="3"/>
-      <c r="E5" s="55"/>
+      <c r="E5" s="57"/>
     </row>
     <row r="6" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="57" t="s">
+      <c r="A6" s="59" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="57"/>
-      <c r="C6" s="57"/>
-      <c r="D6" s="57"/>
-      <c r="E6" s="55"/>
+      <c r="B6" s="59"/>
+      <c r="C6" s="59"/>
+      <c r="D6" s="59"/>
+      <c r="E6" s="57"/>
     </row>
     <row r="7" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="57" t="s">
+      <c r="A7" s="59" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="57"/>
+      <c r="B7" s="59"/>
       <c r="C7" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D7" s="3">
         <v>121112911</v>
       </c>
-      <c r="E7" s="55"/>
+      <c r="E7" s="57"/>
     </row>
     <row r="8" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="58" t="s">
+      <c r="A8" s="60" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="58"/>
-      <c r="C8" s="58"/>
+      <c r="B8" s="60"/>
+      <c r="C8" s="60"/>
       <c r="D8" s="3"/>
-      <c r="E8" s="55"/>
+      <c r="E8" s="57"/>
     </row>
     <row r="9" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="57" t="s">
+      <c r="A9" s="59" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="57"/>
-      <c r="C9" s="57"/>
-      <c r="D9" s="57"/>
-      <c r="E9" s="55"/>
+      <c r="B9" s="59"/>
+      <c r="C9" s="59"/>
+      <c r="D9" s="59"/>
+      <c r="E9" s="57"/>
     </row>
     <row r="10" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="57" t="s">
+      <c r="A10" s="59" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="57"/>
+      <c r="B10" s="59"/>
       <c r="C10" s="3" t="s">
         <v>15</v>
       </c>
       <c r="D10" s="3">
         <v>121112724</v>
       </c>
-      <c r="E10" s="55"/>
+      <c r="E10" s="57"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="53"/>
-      <c r="B11" s="53"/>
-      <c r="C11" s="53"/>
-      <c r="D11" s="54"/>
-      <c r="E11" s="55"/>
+      <c r="A11" s="55"/>
+      <c r="B11" s="55"/>
+      <c r="C11" s="55"/>
+      <c r="D11" s="56"/>
+      <c r="E11" s="57"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -1586,10 +1596,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I79"/>
+  <dimension ref="A1:I83"/>
   <sheetViews>
     <sheetView topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="N72" sqref="N72"/>
+      <selection activeCell="L83" sqref="L83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1598,26 +1608,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="64" t="s">
+      <c r="A1" s="62" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="64"/>
-      <c r="C1" s="64"/>
-      <c r="D1" s="64"/>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
       <c r="F1" s="8"/>
       <c r="G1" s="8"/>
       <c r="H1" s="8"/>
       <c r="I1" s="8"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="65" t="s">
+      <c r="A2" s="64" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="65"/>
-      <c r="C2" s="65"/>
-      <c r="D2" s="65"/>
-      <c r="F2" s="62"/>
-      <c r="G2" s="62"/>
+      <c r="B2" s="64"/>
+      <c r="C2" s="64"/>
+      <c r="D2" s="64"/>
+      <c r="F2" s="65"/>
+      <c r="G2" s="65"/>
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
     </row>
@@ -1909,30 +1919,30 @@
     </row>
     <row r="33" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="5"/>
-      <c r="B33" s="62" t="s">
+      <c r="B33" s="65" t="s">
         <v>30</v>
       </c>
-      <c r="C33" s="62"/>
-      <c r="D33" s="62"/>
+      <c r="C33" s="65"/>
+      <c r="D33" s="65"/>
       <c r="E33" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="66" t="s">
+      <c r="A35" s="68" t="s">
         <v>71</v>
       </c>
-      <c r="B35" s="66"/>
-      <c r="C35" s="66"/>
-      <c r="D35" s="66"/>
+      <c r="B35" s="68"/>
+      <c r="C35" s="68"/>
+      <c r="D35" s="68"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="67" t="s">
+      <c r="A36" s="69" t="s">
         <v>72</v>
       </c>
-      <c r="B36" s="67"/>
-      <c r="C36" s="67"/>
-      <c r="D36" s="67"/>
+      <c r="B36" s="69"/>
+      <c r="C36" s="69"/>
+      <c r="D36" s="69"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="24">
@@ -2185,20 +2195,20 @@
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A64" s="59" t="s">
+      <c r="A64" s="66" t="s">
         <v>96</v>
       </c>
-      <c r="B64" s="59"/>
-      <c r="C64" s="59"/>
-      <c r="D64" s="59"/>
+      <c r="B64" s="66"/>
+      <c r="C64" s="66"/>
+      <c r="D64" s="66"/>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A65" s="60" t="s">
+      <c r="A65" s="67" t="s">
         <v>97</v>
       </c>
-      <c r="B65" s="60"/>
-      <c r="C65" s="60"/>
-      <c r="D65" s="60"/>
+      <c r="B65" s="67"/>
+      <c r="C65" s="67"/>
+      <c r="D65" s="67"/>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="24">
@@ -2320,26 +2330,59 @@
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A79" s="76">
+      <c r="A79" s="24">
         <v>41803</v>
       </c>
-      <c r="B79" s="38"/>
-      <c r="C79" s="38"/>
-      <c r="D79" s="38"/>
+      <c r="B79" s="39"/>
+      <c r="C79" s="39"/>
+      <c r="D79" s="39"/>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" s="39"/>
+      <c r="B80" s="39" t="s">
+        <v>28</v>
+      </c>
+      <c r="C80" s="39"/>
+      <c r="D80" s="39"/>
+      <c r="E80" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" s="39"/>
+      <c r="B81" s="39"/>
+      <c r="C81" s="39"/>
+      <c r="D81" s="39"/>
+      <c r="E81" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" s="39"/>
+      <c r="B82" s="61" t="s">
+        <v>29</v>
+      </c>
+      <c r="C82" s="61"/>
+      <c r="D82" s="61"/>
+      <c r="E82" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83" s="39"/>
+      <c r="B83" s="61" t="s">
+        <v>30</v>
+      </c>
+      <c r="C83" s="61"/>
+      <c r="D83" s="61"/>
+      <c r="E83" t="s">
+        <v>32</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="28">
-    <mergeCell ref="B76:D76"/>
-    <mergeCell ref="B78:D78"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="B24:D24"/>
+  <mergeCells count="30">
+    <mergeCell ref="B82:D82"/>
+    <mergeCell ref="B83:D83"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="A64:D64"/>
     <mergeCell ref="A65:D65"/>
@@ -2356,6 +2399,17 @@
     <mergeCell ref="B49:D49"/>
     <mergeCell ref="B53:D53"/>
     <mergeCell ref="B55:D55"/>
+    <mergeCell ref="B76:D76"/>
+    <mergeCell ref="B78:D78"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="B24:D24"/>
     <mergeCell ref="B59:D59"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2364,29 +2418,29 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M67"/>
+  <dimension ref="A1:M71"/>
   <sheetViews>
-    <sheetView topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="A64" sqref="A64:I67"/>
+    <sheetView topLeftCell="A54" workbookViewId="0">
+      <selection activeCell="I79" sqref="I79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="69" t="s">
+      <c r="A1" s="71" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="70"/>
-      <c r="C1" s="70"/>
-      <c r="D1" s="71"/>
+      <c r="B1" s="72"/>
+      <c r="C1" s="72"/>
+      <c r="D1" s="73"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="72" t="s">
+      <c r="A2" s="74" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="73"/>
-      <c r="C2" s="73"/>
-      <c r="D2" s="74"/>
+      <c r="B2" s="75"/>
+      <c r="C2" s="75"/>
+      <c r="D2" s="76"/>
     </row>
     <row r="3" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="13">
@@ -2398,58 +2452,58 @@
     </row>
     <row r="4" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="15"/>
-      <c r="B4" s="62" t="s">
+      <c r="B4" s="65" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="62"/>
-      <c r="D4" s="62"/>
-      <c r="E4" s="68" t="s">
+      <c r="C4" s="65"/>
+      <c r="D4" s="65"/>
+      <c r="E4" s="70" t="s">
         <v>53</v>
       </c>
-      <c r="F4" s="68"/>
-      <c r="G4" s="68"/>
-      <c r="H4" s="68"/>
-      <c r="I4" s="68"/>
-      <c r="J4" s="68"/>
-      <c r="K4" s="68"/>
+      <c r="F4" s="70"/>
+      <c r="G4" s="70"/>
+      <c r="H4" s="70"/>
+      <c r="I4" s="70"/>
+      <c r="J4" s="70"/>
+      <c r="K4" s="70"/>
     </row>
     <row r="5" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="15"/>
-      <c r="E5" s="68" t="s">
+      <c r="E5" s="70" t="s">
         <v>54</v>
       </c>
-      <c r="F5" s="68"/>
-      <c r="G5" s="68"/>
-      <c r="H5" s="68"/>
-      <c r="I5" s="68"/>
-      <c r="J5" s="68"/>
-      <c r="K5" s="68"/>
+      <c r="F5" s="70"/>
+      <c r="G5" s="70"/>
+      <c r="H5" s="70"/>
+      <c r="I5" s="70"/>
+      <c r="J5" s="70"/>
+      <c r="K5" s="70"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E6" s="68" t="s">
+      <c r="E6" s="70" t="s">
         <v>55</v>
       </c>
-      <c r="F6" s="68"/>
-      <c r="G6" s="68"/>
-      <c r="H6" s="68"/>
-      <c r="I6" s="68"/>
-      <c r="J6" s="68"/>
-      <c r="K6" s="68"/>
+      <c r="F6" s="70"/>
+      <c r="G6" s="70"/>
+      <c r="H6" s="70"/>
+      <c r="I6" s="70"/>
+      <c r="J6" s="70"/>
+      <c r="K6" s="70"/>
     </row>
     <row r="7" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B7" s="62" t="s">
+      <c r="B7" s="65" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="62"/>
-      <c r="D7" s="62"/>
-      <c r="E7" s="68" t="s">
+      <c r="C7" s="65"/>
+      <c r="D7" s="65"/>
+      <c r="E7" s="70" t="s">
         <v>56</v>
       </c>
-      <c r="F7" s="68"/>
-      <c r="G7" s="68"/>
-      <c r="H7" s="68"/>
-      <c r="I7" s="68"/>
-      <c r="J7" s="68"/>
+      <c r="F7" s="70"/>
+      <c r="G7" s="70"/>
+      <c r="H7" s="70"/>
+      <c r="I7" s="70"/>
+      <c r="J7" s="70"/>
     </row>
     <row r="8" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="13">
@@ -2462,37 +2516,37 @@
       </c>
       <c r="C9" s="15"/>
       <c r="D9" s="15"/>
-      <c r="E9" s="68" t="s">
+      <c r="E9" s="70" t="s">
         <v>53</v>
       </c>
-      <c r="F9" s="68"/>
-      <c r="G9" s="68"/>
-      <c r="H9" s="68"/>
-      <c r="I9" s="68"/>
-      <c r="J9" s="68"/>
-      <c r="K9" s="68"/>
+      <c r="F9" s="70"/>
+      <c r="G9" s="70"/>
+      <c r="H9" s="70"/>
+      <c r="I9" s="70"/>
+      <c r="J9" s="70"/>
+      <c r="K9" s="70"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E10" s="68" t="s">
+      <c r="E10" s="70" t="s">
         <v>54</v>
       </c>
-      <c r="F10" s="68"/>
-      <c r="G10" s="68"/>
-      <c r="H10" s="68"/>
-      <c r="I10" s="68"/>
-      <c r="J10" s="68"/>
-      <c r="K10" s="68"/>
+      <c r="F10" s="70"/>
+      <c r="G10" s="70"/>
+      <c r="H10" s="70"/>
+      <c r="I10" s="70"/>
+      <c r="J10" s="70"/>
+      <c r="K10" s="70"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E11" s="68" t="s">
+      <c r="E11" s="70" t="s">
         <v>55</v>
       </c>
-      <c r="F11" s="68"/>
-      <c r="G11" s="68"/>
-      <c r="H11" s="68"/>
-      <c r="I11" s="68"/>
-      <c r="J11" s="68"/>
-      <c r="K11" s="68"/>
+      <c r="F11" s="70"/>
+      <c r="G11" s="70"/>
+      <c r="H11" s="70"/>
+      <c r="I11" s="70"/>
+      <c r="J11" s="70"/>
+      <c r="K11" s="70"/>
     </row>
     <row r="12" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B12" s="15" t="s">
@@ -2500,45 +2554,45 @@
       </c>
       <c r="C12" s="15"/>
       <c r="D12" s="15"/>
-      <c r="E12" s="68" t="s">
+      <c r="E12" s="70" t="s">
         <v>57</v>
       </c>
-      <c r="F12" s="68"/>
-      <c r="G12" s="68"/>
-      <c r="H12" s="68"/>
-      <c r="I12" s="68"/>
-      <c r="J12" s="68"/>
-      <c r="K12" s="68"/>
-      <c r="L12" s="68"/>
-      <c r="M12" s="68"/>
+      <c r="F12" s="70"/>
+      <c r="G12" s="70"/>
+      <c r="H12" s="70"/>
+      <c r="I12" s="70"/>
+      <c r="J12" s="70"/>
+      <c r="K12" s="70"/>
+      <c r="L12" s="70"/>
+      <c r="M12" s="70"/>
     </row>
     <row r="13" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="16"/>
-      <c r="E13" s="68" t="s">
+      <c r="E13" s="70" t="s">
         <v>58</v>
       </c>
-      <c r="F13" s="68"/>
-      <c r="G13" s="68"/>
-      <c r="H13" s="68"/>
-      <c r="I13" s="68"/>
-      <c r="J13" s="68"/>
-      <c r="K13" s="68"/>
-      <c r="L13" s="68"/>
-      <c r="M13" s="68"/>
+      <c r="F13" s="70"/>
+      <c r="G13" s="70"/>
+      <c r="H13" s="70"/>
+      <c r="I13" s="70"/>
+      <c r="J13" s="70"/>
+      <c r="K13" s="70"/>
+      <c r="L13" s="70"/>
+      <c r="M13" s="70"/>
     </row>
     <row r="14" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="15"/>
-      <c r="E14" s="68" t="s">
+      <c r="E14" s="70" t="s">
         <v>59</v>
       </c>
-      <c r="F14" s="68"/>
-      <c r="G14" s="68"/>
-      <c r="H14" s="68"/>
-      <c r="I14" s="68"/>
-      <c r="J14" s="68"/>
-      <c r="K14" s="68"/>
-      <c r="L14" s="68"/>
-      <c r="M14" s="68"/>
+      <c r="F14" s="70"/>
+      <c r="G14" s="70"/>
+      <c r="H14" s="70"/>
+      <c r="I14" s="70"/>
+      <c r="J14" s="70"/>
+      <c r="K14" s="70"/>
+      <c r="L14" s="70"/>
+      <c r="M14" s="70"/>
     </row>
     <row r="15" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="15"/>
@@ -2566,43 +2620,43 @@
       </c>
       <c r="C17" s="15"/>
       <c r="D17" s="15"/>
-      <c r="E17" s="68" t="s">
+      <c r="E17" s="70" t="s">
         <v>57</v>
       </c>
-      <c r="F17" s="68"/>
-      <c r="G17" s="68"/>
-      <c r="H17" s="68"/>
-      <c r="I17" s="68"/>
-      <c r="J17" s="68"/>
-      <c r="K17" s="68"/>
-      <c r="L17" s="68"/>
-      <c r="M17" s="68"/>
+      <c r="F17" s="70"/>
+      <c r="G17" s="70"/>
+      <c r="H17" s="70"/>
+      <c r="I17" s="70"/>
+      <c r="J17" s="70"/>
+      <c r="K17" s="70"/>
+      <c r="L17" s="70"/>
+      <c r="M17" s="70"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E18" s="68" t="s">
+      <c r="E18" s="70" t="s">
         <v>58</v>
       </c>
-      <c r="F18" s="68"/>
-      <c r="G18" s="68"/>
-      <c r="H18" s="68"/>
-      <c r="I18" s="68"/>
-      <c r="J18" s="68"/>
-      <c r="K18" s="68"/>
-      <c r="L18" s="68"/>
-      <c r="M18" s="68"/>
+      <c r="F18" s="70"/>
+      <c r="G18" s="70"/>
+      <c r="H18" s="70"/>
+      <c r="I18" s="70"/>
+      <c r="J18" s="70"/>
+      <c r="K18" s="70"/>
+      <c r="L18" s="70"/>
+      <c r="M18" s="70"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E19" s="68" t="s">
+      <c r="E19" s="70" t="s">
         <v>59</v>
       </c>
-      <c r="F19" s="68"/>
-      <c r="G19" s="68"/>
-      <c r="H19" s="68"/>
-      <c r="I19" s="68"/>
-      <c r="J19" s="68"/>
-      <c r="K19" s="68"/>
-      <c r="L19" s="68"/>
-      <c r="M19" s="68"/>
+      <c r="F19" s="70"/>
+      <c r="G19" s="70"/>
+      <c r="H19" s="70"/>
+      <c r="I19" s="70"/>
+      <c r="J19" s="70"/>
+      <c r="K19" s="70"/>
+      <c r="L19" s="70"/>
+      <c r="M19" s="70"/>
     </row>
     <row r="20" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="15"/>
@@ -2611,10 +2665,10 @@
       </c>
       <c r="C20" s="15"/>
       <c r="D20" s="15"/>
-      <c r="E20" s="68" t="s">
+      <c r="E20" s="70" t="s">
         <v>60</v>
       </c>
-      <c r="F20" s="68"/>
+      <c r="F20" s="70"/>
     </row>
     <row r="21" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="15"/>
@@ -2642,10 +2696,10 @@
       </c>
       <c r="C23" s="15"/>
       <c r="D23" s="15"/>
-      <c r="E23" s="68" t="s">
+      <c r="E23" s="70" t="s">
         <v>60</v>
       </c>
-      <c r="F23" s="68"/>
+      <c r="F23" s="70"/>
     </row>
     <row r="24" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="5"/>
@@ -2670,20 +2724,20 @@
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27" s="66" t="s">
+      <c r="A27" s="68" t="s">
         <v>71</v>
       </c>
-      <c r="B27" s="66"/>
-      <c r="C27" s="66"/>
-      <c r="D27" s="66"/>
+      <c r="B27" s="68"/>
+      <c r="C27" s="68"/>
+      <c r="D27" s="68"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A28" s="67" t="s">
+      <c r="A28" s="69" t="s">
         <v>72</v>
       </c>
-      <c r="B28" s="67"/>
-      <c r="C28" s="67"/>
-      <c r="D28" s="67"/>
+      <c r="B28" s="69"/>
+      <c r="C28" s="69"/>
+      <c r="D28" s="69"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="24">
@@ -2700,18 +2754,18 @@
       </c>
       <c r="C30" s="26"/>
       <c r="D30" s="26"/>
-      <c r="E30" s="68" t="s">
+      <c r="E30" s="70" t="s">
         <v>82</v>
       </c>
-      <c r="F30" s="68"/>
-      <c r="G30" s="68"/>
+      <c r="F30" s="70"/>
+      <c r="G30" s="70"/>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E31" s="68" t="s">
+      <c r="E31" s="70" t="s">
         <v>51</v>
       </c>
-      <c r="F31" s="68"/>
-      <c r="G31" s="68"/>
+      <c r="F31" s="70"/>
+      <c r="G31" s="70"/>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="26"/>
@@ -2739,18 +2793,18 @@
       </c>
       <c r="C34" s="26"/>
       <c r="D34" s="26"/>
-      <c r="E34" s="68" t="s">
+      <c r="E34" s="70" t="s">
         <v>82</v>
       </c>
-      <c r="F34" s="68"/>
-      <c r="G34" s="68"/>
+      <c r="F34" s="70"/>
+      <c r="G34" s="70"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E35" s="68" t="s">
+      <c r="E35" s="70" t="s">
         <v>51</v>
       </c>
-      <c r="F35" s="68"/>
-      <c r="G35" s="68"/>
+      <c r="F35" s="70"/>
+      <c r="G35" s="70"/>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="26"/>
@@ -2759,49 +2813,49 @@
       </c>
       <c r="C36" s="26"/>
       <c r="D36" s="26"/>
-      <c r="E36" s="68" t="s">
+      <c r="E36" s="70" t="s">
         <v>84</v>
       </c>
-      <c r="F36" s="68"/>
-      <c r="G36" s="68"/>
-      <c r="H36" s="68"/>
-      <c r="I36" s="68"/>
-      <c r="J36" s="68"/>
-      <c r="K36" s="68"/>
-      <c r="L36" s="68"/>
+      <c r="F36" s="70"/>
+      <c r="G36" s="70"/>
+      <c r="H36" s="70"/>
+      <c r="I36" s="70"/>
+      <c r="J36" s="70"/>
+      <c r="K36" s="70"/>
+      <c r="L36" s="70"/>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E37" s="68" t="s">
+      <c r="E37" s="70" t="s">
         <v>85</v>
       </c>
-      <c r="F37" s="68"/>
-      <c r="G37" s="68"/>
-      <c r="H37" s="68"/>
-      <c r="I37" s="68"/>
-      <c r="J37" s="68"/>
-      <c r="K37" s="68"/>
+      <c r="F37" s="70"/>
+      <c r="G37" s="70"/>
+      <c r="H37" s="70"/>
+      <c r="I37" s="70"/>
+      <c r="J37" s="70"/>
+      <c r="K37" s="70"/>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E38" s="68" t="s">
+      <c r="E38" s="70" t="s">
         <v>48</v>
       </c>
-      <c r="F38" s="68"/>
-      <c r="G38" s="68"/>
-      <c r="H38" s="68"/>
-      <c r="I38" s="68"/>
-      <c r="J38" s="68"/>
-      <c r="K38" s="68"/>
+      <c r="F38" s="70"/>
+      <c r="G38" s="70"/>
+      <c r="H38" s="70"/>
+      <c r="I38" s="70"/>
+      <c r="J38" s="70"/>
+      <c r="K38" s="70"/>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E39" s="68" t="s">
+      <c r="E39" s="70" t="s">
         <v>86</v>
       </c>
-      <c r="F39" s="68"/>
-      <c r="G39" s="68"/>
-      <c r="H39" s="68"/>
-      <c r="I39" s="68"/>
-      <c r="J39" s="68"/>
-      <c r="K39" s="68"/>
+      <c r="F39" s="70"/>
+      <c r="G39" s="70"/>
+      <c r="H39" s="70"/>
+      <c r="I39" s="70"/>
+      <c r="J39" s="70"/>
+      <c r="K39" s="70"/>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="26"/>
@@ -2810,12 +2864,12 @@
       </c>
       <c r="C40" s="26"/>
       <c r="D40" s="26"/>
-      <c r="E40" s="68" t="s">
+      <c r="E40" s="70" t="s">
         <v>87</v>
       </c>
-      <c r="F40" s="68"/>
-      <c r="G40" s="68"/>
-      <c r="H40" s="68"/>
+      <c r="F40" s="70"/>
+      <c r="G40" s="70"/>
+      <c r="H40" s="70"/>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="24">
@@ -2832,49 +2886,49 @@
       </c>
       <c r="C42" s="26"/>
       <c r="D42" s="26"/>
-      <c r="E42" s="68" t="s">
+      <c r="E42" s="70" t="s">
         <v>84</v>
       </c>
-      <c r="F42" s="68"/>
-      <c r="G42" s="68"/>
-      <c r="H42" s="68"/>
-      <c r="I42" s="68"/>
-      <c r="J42" s="68"/>
-      <c r="K42" s="68"/>
-      <c r="L42" s="68"/>
+      <c r="F42" s="70"/>
+      <c r="G42" s="70"/>
+      <c r="H42" s="70"/>
+      <c r="I42" s="70"/>
+      <c r="J42" s="70"/>
+      <c r="K42" s="70"/>
+      <c r="L42" s="70"/>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E43" s="68" t="s">
+      <c r="E43" s="70" t="s">
         <v>85</v>
       </c>
-      <c r="F43" s="68"/>
-      <c r="G43" s="68"/>
-      <c r="H43" s="68"/>
-      <c r="I43" s="68"/>
-      <c r="J43" s="68"/>
-      <c r="K43" s="68"/>
+      <c r="F43" s="70"/>
+      <c r="G43" s="70"/>
+      <c r="H43" s="70"/>
+      <c r="I43" s="70"/>
+      <c r="J43" s="70"/>
+      <c r="K43" s="70"/>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E44" s="68" t="s">
+      <c r="E44" s="70" t="s">
         <v>48</v>
       </c>
-      <c r="F44" s="68"/>
-      <c r="G44" s="68"/>
-      <c r="H44" s="68"/>
-      <c r="I44" s="68"/>
-      <c r="J44" s="68"/>
-      <c r="K44" s="68"/>
+      <c r="F44" s="70"/>
+      <c r="G44" s="70"/>
+      <c r="H44" s="70"/>
+      <c r="I44" s="70"/>
+      <c r="J44" s="70"/>
+      <c r="K44" s="70"/>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E45" s="68" t="s">
+      <c r="E45" s="70" t="s">
         <v>86</v>
       </c>
-      <c r="F45" s="68"/>
-      <c r="G45" s="68"/>
-      <c r="H45" s="68"/>
-      <c r="I45" s="68"/>
-      <c r="J45" s="68"/>
-      <c r="K45" s="68"/>
+      <c r="F45" s="70"/>
+      <c r="G45" s="70"/>
+      <c r="H45" s="70"/>
+      <c r="I45" s="70"/>
+      <c r="J45" s="70"/>
+      <c r="K45" s="70"/>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="26"/>
@@ -2883,22 +2937,22 @@
       </c>
       <c r="C46" s="26"/>
       <c r="D46" s="26"/>
-      <c r="E46" s="68" t="s">
+      <c r="E46" s="70" t="s">
         <v>62</v>
       </c>
-      <c r="F46" s="68"/>
-      <c r="G46" s="68"/>
-      <c r="H46" s="68"/>
-      <c r="I46" s="68"/>
+      <c r="F46" s="70"/>
+      <c r="G46" s="70"/>
+      <c r="H46" s="70"/>
+      <c r="I46" s="70"/>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E47" s="68" t="s">
+      <c r="E47" s="70" t="s">
         <v>88</v>
       </c>
-      <c r="F47" s="68"/>
-      <c r="G47" s="68"/>
-      <c r="H47" s="68"/>
-      <c r="I47" s="68"/>
+      <c r="F47" s="70"/>
+      <c r="G47" s="70"/>
+      <c r="H47" s="70"/>
+      <c r="I47" s="70"/>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="26"/>
@@ -2907,14 +2961,14 @@
       </c>
       <c r="C48" s="26"/>
       <c r="D48" s="26"/>
-      <c r="E48" s="68" t="s">
+      <c r="E48" s="70" t="s">
         <v>87</v>
       </c>
-      <c r="F48" s="68"/>
-      <c r="G48" s="68"/>
-      <c r="H48" s="68"/>
-      <c r="I48" s="68"/>
-      <c r="J48" s="68"/>
+      <c r="F48" s="70"/>
+      <c r="G48" s="70"/>
+      <c r="H48" s="70"/>
+      <c r="I48" s="70"/>
+      <c r="J48" s="70"/>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="28">
@@ -2931,22 +2985,22 @@
       </c>
       <c r="C50" s="26"/>
       <c r="D50" s="26"/>
-      <c r="E50" s="68" t="s">
+      <c r="E50" s="70" t="s">
         <v>62</v>
       </c>
-      <c r="F50" s="68"/>
-      <c r="G50" s="68"/>
-      <c r="H50" s="68"/>
-      <c r="I50" s="68"/>
+      <c r="F50" s="70"/>
+      <c r="G50" s="70"/>
+      <c r="H50" s="70"/>
+      <c r="I50" s="70"/>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="E51" s="68" t="s">
+      <c r="E51" s="70" t="s">
         <v>88</v>
       </c>
-      <c r="F51" s="68"/>
-      <c r="G51" s="68"/>
-      <c r="H51" s="68"/>
-      <c r="I51" s="68"/>
+      <c r="F51" s="70"/>
+      <c r="G51" s="70"/>
+      <c r="H51" s="70"/>
+      <c r="I51" s="70"/>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="25"/>
@@ -2955,22 +3009,22 @@
       </c>
       <c r="C52" s="26"/>
       <c r="D52" s="26"/>
-      <c r="E52" s="68" t="s">
+      <c r="E52" s="70" t="s">
         <v>62</v>
       </c>
-      <c r="F52" s="68"/>
-      <c r="G52" s="68"/>
-      <c r="H52" s="68"/>
-      <c r="I52" s="68"/>
+      <c r="F52" s="70"/>
+      <c r="G52" s="70"/>
+      <c r="H52" s="70"/>
+      <c r="I52" s="70"/>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="E53" s="68" t="s">
+      <c r="E53" s="70" t="s">
         <v>88</v>
       </c>
-      <c r="F53" s="68"/>
-      <c r="G53" s="68"/>
-      <c r="H53" s="68"/>
-      <c r="I53" s="68"/>
+      <c r="F53" s="70"/>
+      <c r="G53" s="70"/>
+      <c r="H53" s="70"/>
+      <c r="I53" s="70"/>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="25"/>
@@ -2979,30 +3033,30 @@
       </c>
       <c r="C54" s="26"/>
       <c r="D54" s="26"/>
-      <c r="E54" s="68" t="s">
+      <c r="E54" s="70" t="s">
         <v>87</v>
       </c>
-      <c r="F54" s="68"/>
-      <c r="G54" s="68"/>
-      <c r="H54" s="68"/>
-      <c r="I54" s="68"/>
-      <c r="J54" s="68"/>
+      <c r="F54" s="70"/>
+      <c r="G54" s="70"/>
+      <c r="H54" s="70"/>
+      <c r="I54" s="70"/>
+      <c r="J54" s="70"/>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A56" s="59" t="s">
+      <c r="A56" s="66" t="s">
         <v>96</v>
       </c>
-      <c r="B56" s="59"/>
-      <c r="C56" s="59"/>
-      <c r="D56" s="59"/>
+      <c r="B56" s="66"/>
+      <c r="C56" s="66"/>
+      <c r="D56" s="66"/>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A57" s="60" t="s">
+      <c r="A57" s="67" t="s">
         <v>97</v>
       </c>
-      <c r="B57" s="60"/>
-      <c r="C57" s="60"/>
-      <c r="D57" s="60"/>
+      <c r="B57" s="67"/>
+      <c r="C57" s="67"/>
+      <c r="D57" s="67"/>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="24">
@@ -3017,23 +3071,23 @@
       <c r="B59" t="s">
         <v>28</v>
       </c>
-      <c r="E59" s="68" t="s">
+      <c r="E59" s="70" t="s">
         <v>62</v>
       </c>
-      <c r="F59" s="68"/>
-      <c r="G59" s="68"/>
-      <c r="H59" s="68"/>
-      <c r="I59" s="68"/>
+      <c r="F59" s="70"/>
+      <c r="G59" s="70"/>
+      <c r="H59" s="70"/>
+      <c r="I59" s="70"/>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="27"/>
-      <c r="E60" s="68" t="s">
+      <c r="E60" s="70" t="s">
         <v>88</v>
       </c>
-      <c r="F60" s="68"/>
-      <c r="G60" s="68"/>
-      <c r="H60" s="68"/>
-      <c r="I60" s="68"/>
+      <c r="F60" s="70"/>
+      <c r="G60" s="70"/>
+      <c r="H60" s="70"/>
+      <c r="I60" s="70"/>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="27"/>
@@ -3104,38 +3158,49 @@
         <v>101</v>
       </c>
     </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" s="24">
+        <v>41803</v>
+      </c>
+      <c r="B68" s="39"/>
+      <c r="C68" s="39"/>
+      <c r="D68" s="39"/>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" s="39"/>
+      <c r="B69" s="39" t="s">
+        <v>28</v>
+      </c>
+      <c r="C69" s="39"/>
+      <c r="D69" s="39"/>
+      <c r="E69" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" s="39"/>
+      <c r="B70" s="39" t="s">
+        <v>29</v>
+      </c>
+      <c r="C70" s="39"/>
+      <c r="D70" s="39"/>
+      <c r="E70" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" s="39"/>
+      <c r="B71" s="39" t="s">
+        <v>30</v>
+      </c>
+      <c r="C71" s="39"/>
+      <c r="D71" s="39"/>
+      <c r="E71" t="s">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="46">
-    <mergeCell ref="E44:K44"/>
-    <mergeCell ref="E45:K45"/>
-    <mergeCell ref="E52:I52"/>
-    <mergeCell ref="E53:I53"/>
-    <mergeCell ref="E54:J54"/>
-    <mergeCell ref="E46:I46"/>
-    <mergeCell ref="E47:I47"/>
-    <mergeCell ref="E48:J48"/>
-    <mergeCell ref="E50:I50"/>
-    <mergeCell ref="E51:I51"/>
-    <mergeCell ref="E38:K38"/>
-    <mergeCell ref="E39:K39"/>
-    <mergeCell ref="E40:H40"/>
-    <mergeCell ref="E42:L42"/>
-    <mergeCell ref="E43:K43"/>
-    <mergeCell ref="E31:G31"/>
-    <mergeCell ref="E34:G34"/>
-    <mergeCell ref="E35:G35"/>
-    <mergeCell ref="E36:L36"/>
-    <mergeCell ref="E37:K37"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="E4:K4"/>
-    <mergeCell ref="E5:K5"/>
-    <mergeCell ref="E6:K6"/>
-    <mergeCell ref="E7:J7"/>
-    <mergeCell ref="E9:K9"/>
-    <mergeCell ref="E10:K10"/>
-    <mergeCell ref="E11:K11"/>
     <mergeCell ref="E59:I59"/>
     <mergeCell ref="E60:I60"/>
     <mergeCell ref="A56:D56"/>
@@ -3152,6 +3217,36 @@
     <mergeCell ref="A27:D27"/>
     <mergeCell ref="A28:D28"/>
     <mergeCell ref="E30:G30"/>
+    <mergeCell ref="E6:K6"/>
+    <mergeCell ref="E7:J7"/>
+    <mergeCell ref="E9:K9"/>
+    <mergeCell ref="E10:K10"/>
+    <mergeCell ref="E11:K11"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="E4:K4"/>
+    <mergeCell ref="E5:K5"/>
+    <mergeCell ref="E31:G31"/>
+    <mergeCell ref="E34:G34"/>
+    <mergeCell ref="E35:G35"/>
+    <mergeCell ref="E36:L36"/>
+    <mergeCell ref="E37:K37"/>
+    <mergeCell ref="E38:K38"/>
+    <mergeCell ref="E39:K39"/>
+    <mergeCell ref="E40:H40"/>
+    <mergeCell ref="E42:L42"/>
+    <mergeCell ref="E43:K43"/>
+    <mergeCell ref="E44:K44"/>
+    <mergeCell ref="E45:K45"/>
+    <mergeCell ref="E52:I52"/>
+    <mergeCell ref="E53:I53"/>
+    <mergeCell ref="E54:J54"/>
+    <mergeCell ref="E46:I46"/>
+    <mergeCell ref="E47:I47"/>
+    <mergeCell ref="E48:J48"/>
+    <mergeCell ref="E50:I50"/>
+    <mergeCell ref="E51:I51"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3159,29 +3254,29 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O71"/>
+  <dimension ref="A1:O75"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="A68" sqref="A68:H71"/>
+      <selection activeCell="F76" sqref="F76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="64" t="s">
+      <c r="A1" s="62" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="64"/>
-      <c r="C1" s="64"/>
-      <c r="D1" s="64"/>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="65" t="s">
+      <c r="A2" s="64" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="65"/>
-      <c r="C2" s="65"/>
-      <c r="D2" s="65"/>
+      <c r="B2" s="64"/>
+      <c r="C2" s="64"/>
+      <c r="D2" s="64"/>
     </row>
     <row r="3" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="20">
@@ -3247,17 +3342,17 @@
       </c>
       <c r="C9" s="18"/>
       <c r="D9" s="18"/>
-      <c r="E9" s="68" t="s">
+      <c r="E9" s="70" t="s">
         <v>64</v>
       </c>
-      <c r="F9" s="68"/>
-      <c r="G9" s="68"/>
-      <c r="H9" s="68"/>
-      <c r="I9" s="68"/>
-      <c r="J9" s="68"/>
-      <c r="K9" s="68"/>
-      <c r="L9" s="68"/>
-      <c r="M9" s="68"/>
+      <c r="F9" s="70"/>
+      <c r="G9" s="70"/>
+      <c r="H9" s="70"/>
+      <c r="I9" s="70"/>
+      <c r="J9" s="70"/>
+      <c r="K9" s="70"/>
+      <c r="L9" s="70"/>
+      <c r="M9" s="70"/>
     </row>
     <row r="10" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="17"/>
@@ -3290,16 +3385,16 @@
       <c r="B13" s="18"/>
       <c r="C13" s="18"/>
       <c r="D13" s="18"/>
-      <c r="E13" s="68" t="s">
+      <c r="E13" s="70" t="s">
         <v>66</v>
       </c>
-      <c r="F13" s="68"/>
-      <c r="G13" s="68"/>
-      <c r="H13" s="68"/>
-      <c r="I13" s="68"/>
-      <c r="J13" s="68"/>
-      <c r="K13" s="68"/>
-      <c r="L13" s="68"/>
+      <c r="F13" s="70"/>
+      <c r="G13" s="70"/>
+      <c r="H13" s="70"/>
+      <c r="I13" s="70"/>
+      <c r="J13" s="70"/>
+      <c r="K13" s="70"/>
+      <c r="L13" s="70"/>
     </row>
     <row r="14" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="17"/>
@@ -3325,45 +3420,45 @@
     </row>
     <row r="17" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="17"/>
-      <c r="B17" s="62" t="s">
+      <c r="B17" s="65" t="s">
         <v>28</v>
       </c>
-      <c r="C17" s="62"/>
-      <c r="D17" s="62"/>
-      <c r="E17" s="68" t="s">
+      <c r="C17" s="65"/>
+      <c r="D17" s="65"/>
+      <c r="E17" s="70" t="s">
         <v>67</v>
       </c>
-      <c r="F17" s="68"/>
-      <c r="G17" s="68"/>
-      <c r="H17" s="68"/>
-      <c r="I17" s="68"/>
-      <c r="J17" s="68"/>
-      <c r="K17" s="68"/>
+      <c r="F17" s="70"/>
+      <c r="G17" s="70"/>
+      <c r="H17" s="70"/>
+      <c r="I17" s="70"/>
+      <c r="J17" s="70"/>
+      <c r="K17" s="70"/>
     </row>
     <row r="18" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="17"/>
       <c r="B18" s="18"/>
       <c r="C18" s="18"/>
       <c r="D18" s="18"/>
-      <c r="E18" s="68" t="s">
+      <c r="E18" s="70" t="s">
         <v>68</v>
       </c>
-      <c r="F18" s="68"/>
-      <c r="G18" s="68"/>
-      <c r="H18" s="68"/>
-      <c r="I18" s="68"/>
-      <c r="J18" s="68"/>
-      <c r="K18" s="68"/>
+      <c r="F18" s="70"/>
+      <c r="G18" s="70"/>
+      <c r="H18" s="70"/>
+      <c r="I18" s="70"/>
+      <c r="J18" s="70"/>
+      <c r="K18" s="70"/>
     </row>
     <row r="19" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="17"/>
       <c r="B19" s="18"/>
       <c r="C19" s="18"/>
       <c r="D19" s="18"/>
-      <c r="E19" s="68" t="s">
+      <c r="E19" s="70" t="s">
         <v>41</v>
       </c>
-      <c r="F19" s="68"/>
+      <c r="F19" s="70"/>
     </row>
     <row r="20" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="17"/>
@@ -3378,29 +3473,29 @@
       </c>
       <c r="C21" s="63"/>
       <c r="D21" s="63"/>
-      <c r="E21" s="68" t="s">
+      <c r="E21" s="70" t="s">
         <v>45</v>
       </c>
-      <c r="F21" s="68"/>
-      <c r="G21" s="68"/>
-      <c r="H21" s="68"/>
-      <c r="I21" s="68"/>
-      <c r="J21" s="68"/>
-      <c r="K21" s="68"/>
-      <c r="L21" s="68"/>
-      <c r="M21" s="68"/>
-      <c r="N21" s="68"/>
-      <c r="O21" s="68"/>
+      <c r="F21" s="70"/>
+      <c r="G21" s="70"/>
+      <c r="H21" s="70"/>
+      <c r="I21" s="70"/>
+      <c r="J21" s="70"/>
+      <c r="K21" s="70"/>
+      <c r="L21" s="70"/>
+      <c r="M21" s="70"/>
+      <c r="N21" s="70"/>
+      <c r="O21" s="70"/>
     </row>
     <row r="22" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="17"/>
       <c r="B22" s="18"/>
       <c r="C22" s="18"/>
       <c r="D22" s="18"/>
-      <c r="E22" s="68" t="s">
+      <c r="E22" s="70" t="s">
         <v>69</v>
       </c>
-      <c r="F22" s="68"/>
+      <c r="F22" s="70"/>
     </row>
     <row r="23" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="17"/>
@@ -3451,55 +3546,55 @@
       </c>
       <c r="C28" s="63"/>
       <c r="D28" s="63"/>
-      <c r="E28" s="68" t="s">
+      <c r="E28" s="70" t="s">
         <v>62</v>
       </c>
-      <c r="F28" s="68"/>
-      <c r="G28" s="68"/>
-      <c r="H28" s="68"/>
+      <c r="F28" s="70"/>
+      <c r="G28" s="70"/>
+      <c r="H28" s="70"/>
     </row>
     <row r="29" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="5"/>
       <c r="B29" s="18"/>
       <c r="C29" s="18"/>
       <c r="D29" s="18"/>
-      <c r="E29" s="68"/>
-      <c r="F29" s="68"/>
+      <c r="E29" s="70"/>
+      <c r="F29" s="70"/>
     </row>
     <row r="30" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="5"/>
-      <c r="B30" s="62" t="s">
+      <c r="B30" s="65" t="s">
         <v>30</v>
       </c>
-      <c r="C30" s="62"/>
-      <c r="D30" s="62"/>
-      <c r="E30" s="75" t="s">
+      <c r="C30" s="65"/>
+      <c r="D30" s="65"/>
+      <c r="E30" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F30" s="75"/>
-      <c r="G30" s="75"/>
+      <c r="F30" s="77"/>
+      <c r="G30" s="77"/>
     </row>
     <row r="31" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="5"/>
-      <c r="B31" s="62"/>
-      <c r="C31" s="62"/>
-      <c r="D31" s="62"/>
+      <c r="B31" s="65"/>
+      <c r="C31" s="65"/>
+      <c r="D31" s="65"/>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A32" s="66" t="s">
+      <c r="A32" s="68" t="s">
         <v>71</v>
       </c>
-      <c r="B32" s="66"/>
-      <c r="C32" s="66"/>
-      <c r="D32" s="66"/>
+      <c r="B32" s="68"/>
+      <c r="C32" s="68"/>
+      <c r="D32" s="68"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="67" t="s">
+      <c r="A33" s="69" t="s">
         <v>72</v>
       </c>
-      <c r="B33" s="67"/>
-      <c r="C33" s="67"/>
-      <c r="D33" s="67"/>
+      <c r="B33" s="69"/>
+      <c r="C33" s="69"/>
+      <c r="D33" s="69"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="31">
@@ -3516,23 +3611,23 @@
       </c>
       <c r="C35" s="61"/>
       <c r="D35" s="61"/>
-      <c r="E35" s="68" t="s">
+      <c r="E35" s="70" t="s">
         <v>89</v>
       </c>
-      <c r="F35" s="68"/>
-      <c r="G35" s="68"/>
-      <c r="H35" s="68"/>
-      <c r="I35" s="68"/>
+      <c r="F35" s="70"/>
+      <c r="G35" s="70"/>
+      <c r="H35" s="70"/>
+      <c r="I35" s="70"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="32"/>
       <c r="B36" s="61"/>
       <c r="C36" s="61"/>
       <c r="D36" s="61"/>
-      <c r="E36" s="68" t="s">
+      <c r="E36" s="70" t="s">
         <v>51</v>
       </c>
-      <c r="F36" s="68"/>
+      <c r="F36" s="70"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="33"/>
@@ -3718,15 +3813,15 @@
       <c r="B54" s="26"/>
       <c r="C54" s="26"/>
       <c r="D54" s="26"/>
-      <c r="E54" s="68" t="s">
+      <c r="E54" s="70" t="s">
         <v>94</v>
       </c>
-      <c r="F54" s="68"/>
-      <c r="G54" s="68"/>
-      <c r="H54" s="68"/>
-      <c r="I54" s="68"/>
-      <c r="J54" s="68"/>
-      <c r="K54" s="68"/>
+      <c r="F54" s="70"/>
+      <c r="G54" s="70"/>
+      <c r="H54" s="70"/>
+      <c r="I54" s="70"/>
+      <c r="J54" s="70"/>
+      <c r="K54" s="70"/>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="25"/>
@@ -3755,20 +3850,20 @@
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A59" s="59" t="s">
+      <c r="A59" s="66" t="s">
         <v>96</v>
       </c>
-      <c r="B59" s="59"/>
-      <c r="C59" s="59"/>
-      <c r="D59" s="59"/>
+      <c r="B59" s="66"/>
+      <c r="C59" s="66"/>
+      <c r="D59" s="66"/>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A60" s="60" t="s">
+      <c r="A60" s="67" t="s">
         <v>97</v>
       </c>
-      <c r="B60" s="60"/>
-      <c r="C60" s="60"/>
-      <c r="D60" s="60"/>
+      <c r="B60" s="67"/>
+      <c r="C60" s="67"/>
+      <c r="D60" s="67"/>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="24">
@@ -3783,29 +3878,29 @@
       <c r="B62" t="s">
         <v>28</v>
       </c>
-      <c r="E62" s="68" t="s">
+      <c r="E62" s="70" t="s">
         <v>102</v>
       </c>
-      <c r="F62" s="68"/>
+      <c r="F62" s="70"/>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="27"/>
-      <c r="E63" s="68" t="s">
+      <c r="E63" s="70" t="s">
         <v>103</v>
       </c>
-      <c r="F63" s="68"/>
-      <c r="G63" s="68"/>
+      <c r="F63" s="70"/>
+      <c r="G63" s="70"/>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="27"/>
-      <c r="E64" s="68" t="s">
+      <c r="E64" s="70" t="s">
         <v>104</v>
       </c>
-      <c r="F64" s="68"/>
-      <c r="G64" s="68"/>
-      <c r="H64" s="68"/>
-      <c r="I64" s="68"/>
-      <c r="J64" s="68"/>
+      <c r="F64" s="70"/>
+      <c r="G64" s="70"/>
+      <c r="H64" s="70"/>
+      <c r="I64" s="70"/>
+      <c r="J64" s="70"/>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="27"/>
@@ -3814,11 +3909,11 @@
       </c>
       <c r="C65" s="61"/>
       <c r="D65" s="61"/>
-      <c r="E65" s="68" t="s">
+      <c r="E65" s="70" t="s">
         <v>99</v>
       </c>
-      <c r="F65" s="68"/>
-      <c r="G65" s="68"/>
+      <c r="F65" s="70"/>
+      <c r="G65" s="70"/>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="27"/>
@@ -3862,11 +3957,11 @@
       </c>
       <c r="C70" s="61"/>
       <c r="D70" s="61"/>
-      <c r="E70" s="68" t="s">
+      <c r="E70" s="70" t="s">
         <v>107</v>
       </c>
-      <c r="F70" s="68"/>
-      <c r="G70" s="68"/>
+      <c r="F70" s="70"/>
+      <c r="G70" s="70"/>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="38"/>
@@ -3879,8 +3974,68 @@
         <v>108</v>
       </c>
     </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A72" s="40">
+        <v>41803</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B73" t="s">
+        <v>28</v>
+      </c>
+      <c r="E73" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B74" t="s">
+        <v>29</v>
+      </c>
+      <c r="E74" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B75" t="s">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="50">
+    <mergeCell ref="B65:D65"/>
+    <mergeCell ref="E65:G65"/>
+    <mergeCell ref="B67:D67"/>
+    <mergeCell ref="A59:D59"/>
+    <mergeCell ref="A60:D60"/>
+    <mergeCell ref="E62:F62"/>
+    <mergeCell ref="E63:G63"/>
+    <mergeCell ref="E64:J64"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="E21:O21"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="E28:H28"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="E30:G30"/>
+    <mergeCell ref="E9:M9"/>
+    <mergeCell ref="E13:L13"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="E17:K17"/>
+    <mergeCell ref="E18:K18"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A32:D32"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B6:D6"/>
     <mergeCell ref="B70:D70"/>
     <mergeCell ref="E70:G70"/>
     <mergeCell ref="B71:D71"/>
@@ -3897,40 +4052,6 @@
     <mergeCell ref="E54:K54"/>
     <mergeCell ref="B40:D40"/>
     <mergeCell ref="B35:D35"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A32:D32"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="E9:M9"/>
-    <mergeCell ref="E13:L13"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="E17:K17"/>
-    <mergeCell ref="E18:K18"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="E21:O21"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="E28:H28"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="E30:G30"/>
-    <mergeCell ref="B65:D65"/>
-    <mergeCell ref="E65:G65"/>
-    <mergeCell ref="B67:D67"/>
-    <mergeCell ref="A59:D59"/>
-    <mergeCell ref="A60:D60"/>
-    <mergeCell ref="E62:F62"/>
-    <mergeCell ref="E63:G63"/>
-    <mergeCell ref="E64:J64"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>